<commit_message>
capture more dummy data
</commit_message>
<xml_diff>
--- a/tests/_dummy_data.xlsx
+++ b/tests/_dummy_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC98D501-2F80-413E-8D48-47650BF42FB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE58D750-728B-4E7F-B965-F035982271DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="398">
   <si>
     <t xml:space="preserve">Semiology </t>
   </si>
@@ -1222,6 +1222,27 @@
   </si>
   <si>
     <t>Romagnoli et al on paediatric frontal lobe recordings 2025</t>
+  </si>
+  <si>
+    <t>ADNFLE</t>
+  </si>
+  <si>
+    <t>anonymous, ADNFLE</t>
+  </si>
+  <si>
+    <t>leg bicycling</t>
+  </si>
+  <si>
+    <t>Hypermotor</t>
+  </si>
+  <si>
+    <t>SPECT</t>
+  </si>
+  <si>
+    <t>concordant ictal SPECT and sEEG</t>
+  </si>
+  <si>
+    <t>frontal, cingulate</t>
   </si>
 </sst>
 </file>
@@ -2768,46 +2789,46 @@
                   <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>2</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>91</c:v>
@@ -2993,7 +3014,7 @@
                   <c:v>454</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>477</c:v>
@@ -3002,64 +3023,64 @@
                   <c:v>480</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>564</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3443,73 +3464,73 @@
                   <c:v>1041</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1119.5</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1357.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4666,10 +4687,10 @@
   <dimension ref="A1:DU51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="CY3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="CZ3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="DG10" sqref="DG10"/>
+      <selection pane="bottomRight" activeCell="DE7" sqref="DE7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5392,14 +5413,74 @@
       <c r="DT6" s="34"/>
       <c r="DU6" s="34"/>
     </row>
-    <row r="7" spans="1:125">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
+    <row r="7" spans="1:125" ht="30">
+      <c r="A7" s="33" t="s">
+        <v>392</v>
+      </c>
+      <c r="B7" s="33">
+        <v>10</v>
+      </c>
+      <c r="C7" s="33">
+        <v>10</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>393</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>394</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>396</v>
+      </c>
       <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
+      <c r="H7" s="33" t="s">
+        <v>395</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="M7" s="5">
+        <v>10</v>
+      </c>
+      <c r="P7" s="5">
+        <v>10</v>
+      </c>
+      <c r="Q7" s="32" t="s">
+        <v>397</v>
+      </c>
+      <c r="AL7" s="5">
+        <v>10</v>
+      </c>
+      <c r="AN7" s="5">
+        <v>5</v>
+      </c>
+      <c r="AV7" s="5">
+        <v>5</v>
+      </c>
+      <c r="AW7" s="5">
+        <v>1</v>
+      </c>
+      <c r="BQ7" s="5">
+        <v>2</v>
+      </c>
+      <c r="BS7" s="5">
+        <v>2</v>
+      </c>
+      <c r="DA7" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="DB7" s="6">
+        <v>10</v>
+      </c>
+      <c r="DC7" s="6">
+        <v>0</v>
+      </c>
+      <c r="DD7" s="5">
+        <v>0</v>
+      </c>
+      <c r="DH7" s="5" t="s">
+        <v>391</v>
+      </c>
       <c r="DP7" s="34"/>
       <c r="DQ7" s="34"/>
       <c r="DR7" s="34"/>
@@ -7166,11 +7247,11 @@
       </c>
       <c r="D6" s="40">
         <f>COUNTA(Main!A2:A47)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" s="40">
         <f>SUM(Main!C2:C47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F6" s="40">
         <f>SUM(Main!J2:J47)</f>
@@ -7178,7 +7259,7 @@
       </c>
       <c r="G6" s="40">
         <f>SUM(Main!P2:P47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="40" customFormat="1">
@@ -7194,7 +7275,7 @@
       </c>
       <c r="D7" s="40">
         <f>COUNTA(Main!A3:A47)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" s="40">
         <v>477</v>
@@ -7222,7 +7303,7 @@
       </c>
       <c r="D8" s="40">
         <f>COUNTA(Main!A2:A47)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E8" s="40">
         <v>480</v>
@@ -7233,7 +7314,7 @@
       </c>
       <c r="G8" s="62">
         <f>SUM(Main!$P$2:P47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="40" customFormat="1">
@@ -7249,11 +7330,11 @@
       </c>
       <c r="D9" s="40">
         <f>COUNTA(Main!$A$2:A47)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E9" s="40">
         <f>SUM(Main!$C$2:C47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F9" s="40">
         <f>SUM(Main!$J$2:J47)</f>
@@ -7261,7 +7342,7 @@
       </c>
       <c r="G9" s="40">
         <f>SUM(Main!$P$2:P47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:13" s="40" customFormat="1">
@@ -7277,11 +7358,11 @@
       </c>
       <c r="D10" s="40">
         <f>COUNTA(Main!$A$2:A47)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E10" s="40">
         <f>SUM(Main!$C$2:C47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F10" s="40">
         <f>SUM(Main!$J$2:J47)</f>
@@ -7289,7 +7370,7 @@
       </c>
       <c r="G10" s="40">
         <f>SUM(Main!$P$2:P47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="40" customFormat="1">
@@ -7305,11 +7386,11 @@
       </c>
       <c r="D11" s="40">
         <f>COUNTA(Main!$A$2:A47)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E11" s="40">
         <f>SUM(Main!$C$2:C47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F11" s="40">
         <f>SUM(Main!$J$2:J47)</f>
@@ -7317,7 +7398,7 @@
       </c>
       <c r="G11" s="40">
         <f>SUM(Main!$P$2:P47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -7356,11 +7437,11 @@
       </c>
       <c r="D13" s="40">
         <f>COUNTA(Main!$A$2:A47)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E13" s="40">
         <f>SUM(Main!$C$2:C47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F13" s="40">
         <f>SUM(Main!$J$2:J47)</f>
@@ -7368,7 +7449,7 @@
       </c>
       <c r="G13" s="40">
         <f>SUM(Main!$P$2:P47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="40" customFormat="1">
@@ -7386,7 +7467,7 @@
       </c>
       <c r="E14" s="40">
         <f>SUM(Main!$C$2:C47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F14" s="40">
         <f>SUM(Main!$J$2:J47)</f>
@@ -7394,7 +7475,7 @@
       </c>
       <c r="G14" s="40">
         <f>SUM(Main!$P$2:P47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="40" customFormat="1">
@@ -7410,11 +7491,11 @@
       </c>
       <c r="D15" s="40">
         <f>COUNTA(Main!$A$2:A47)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E15" s="40">
         <f>SUM(Main!$C$2:C47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F15" s="40">
         <f>SUM(Main!$J$2:J47)</f>
@@ -7422,7 +7503,7 @@
       </c>
       <c r="G15" s="40">
         <f>SUM(Main!$P$2:P47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="40" customFormat="1">
@@ -7438,11 +7519,11 @@
       </c>
       <c r="D16" s="40">
         <f>COUNTA(Main!$A$2:A47)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E16" s="40">
         <f>SUM(Main!$C$2:C47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F16" s="40">
         <f>SUM(Main!$J$2:J47)</f>
@@ -7450,7 +7531,7 @@
       </c>
       <c r="G16" s="40">
         <f>SUM(Main!$P$2:P47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -7466,11 +7547,11 @@
       </c>
       <c r="D17" s="40">
         <f>COUNTA(Main!$A$2:A47)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E17" s="40">
         <f>SUM(Main!$C$2:C47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F17" s="40">
         <f>SUM(Main!$J$2:J47)</f>
@@ -7478,7 +7559,7 @@
       </c>
       <c r="G17" s="40">
         <f>SUM(Main!$P$2:P47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -7494,11 +7575,11 @@
       </c>
       <c r="D18" s="40">
         <f>COUNTA(Main!$A$2:A47)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E18" s="40">
         <f>SUM(Main!$C$2:C47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F18" s="40">
         <f>SUM(Main!$J$2:J47)</f>
@@ -7506,7 +7587,7 @@
       </c>
       <c r="G18" s="40">
         <f>SUM(Main!$P$2:P47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -7521,11 +7602,11 @@
       </c>
       <c r="D19" s="40">
         <f>COUNTA(Main!$A$2:A47)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E19" s="40">
         <f>SUM(Main!$C$2:C47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F19" s="40">
         <f>SUM(Main!$J$2:J47)</f>
@@ -7533,7 +7614,7 @@
       </c>
       <c r="G19" s="40">
         <f>SUM(Main!$P$2:P47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -7551,7 +7632,7 @@
       </c>
       <c r="E20" s="40">
         <f>SUM(Main!$C$2:C47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F20" s="40">
         <f>SUM(Main!$J$2:J47)</f>
@@ -7559,7 +7640,7 @@
       </c>
       <c r="G20" s="40">
         <f>SUM(Main!$P$2:P47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -7577,7 +7658,7 @@
       </c>
       <c r="E21" s="40">
         <f>SUM(Main!$C$2:C47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F21" s="40">
         <f>SUM(Main!$J$2:J47)</f>
@@ -7585,7 +7666,7 @@
       </c>
       <c r="G21" s="40">
         <f>SUM(Main!$P$2:P47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -7603,7 +7684,7 @@
       </c>
       <c r="E22" s="40">
         <f>SUM(Main!$C$2:C47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F22" s="40">
         <f>SUM(Main!$J$2:J47)</f>
@@ -7611,7 +7692,7 @@
       </c>
       <c r="G22" s="40">
         <f>SUM(Main!$P$2:P47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -7629,7 +7710,7 @@
       </c>
       <c r="E23" s="40">
         <f>SUM(Main!$C$2:C47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F23" s="40">
         <f>SUM(Main!$J$2:J47)</f>
@@ -7637,7 +7718,7 @@
       </c>
       <c r="G23" s="40">
         <f>SUM(Main!$P$2:P47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -7655,7 +7736,7 @@
       </c>
       <c r="E24" s="40">
         <f>SUM(Main!$C$2:C47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F24" s="40">
         <f>SUM(Main!$J$2:J47)</f>
@@ -7663,7 +7744,7 @@
       </c>
       <c r="G24" s="40">
         <f>SUM(Main!$P$2:P47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -7681,7 +7762,7 @@
       </c>
       <c r="E25" s="40">
         <f>SUM(Main!$C$2:C47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F25" s="40">
         <f>SUM(Main!$J$2:J47)</f>
@@ -7689,7 +7770,7 @@
       </c>
       <c r="G25" s="40">
         <f>SUM(Main!$P$2:P47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -7707,7 +7788,7 @@
       </c>
       <c r="E26" s="40">
         <f>SUM(Main!$C$2:C47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F26" s="40">
         <f>SUM(Main!$J$2:J47)</f>
@@ -7715,7 +7796,7 @@
       </c>
       <c r="G26" s="40">
         <f>SUM(Main!$P$2:P47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="H26" t="s">
         <v>139</v>
@@ -7737,7 +7818,7 @@
       </c>
       <c r="E27" s="40">
         <f>SUM(Main!$C$2:C47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F27" s="40">
         <f>SUM(Main!$J$2:J47)</f>
@@ -7745,7 +7826,7 @@
       </c>
       <c r="G27" s="40">
         <f>SUM(Main!$P$2:P47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -7763,7 +7844,7 @@
       </c>
       <c r="E28" s="40">
         <f>SUM(Main!$C$2:C47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F28" s="40">
         <f>SUM(Main!$J$2:J47)</f>
@@ -7771,7 +7852,7 @@
       </c>
       <c r="G28" s="40">
         <f>SUM(Main!$P$2:P47)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="H28" t="s">
         <v>140</v>

</xml_diff>

<commit_message>
dummy data CES entry
</commit_message>
<xml_diff>
--- a/tests/_dummy_data.xlsx
+++ b/tests/_dummy_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE58D750-728B-4E7F-B965-F035982271DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2E5CF1-1995-41DA-A2FB-A5095AA889CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="398">
   <si>
     <t xml:space="preserve">Semiology </t>
   </si>
@@ -4690,7 +4690,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="CZ3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="DE7" sqref="DE7"/>
+      <selection pane="bottomRight" activeCell="DE11" sqref="DE11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5478,6 +5478,9 @@
       <c r="DD7" s="5">
         <v>0</v>
       </c>
+      <c r="DE7" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="DH7" s="5" t="s">
         <v>391</v>
       </c>

</xml_diff>

<commit_message>
test_dymmy_data: default exclusions & granular
</commit_message>
<xml_diff>
--- a/tests/_dummy_data.xlsx
+++ b/tests/_dummy_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4F29AA-3B2F-4E76-9C94-7264410CCEF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D9372A-904E-4EC0-B130-0F67D2386BB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -2313,10 +2313,10 @@
   <dimension ref="A1:DU51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D27" sqref="D27:E27"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -6304,7 +6304,7 @@
   <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -6323,484 +6323,275 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="109">
+      <c r="A2">
         <v>32</v>
       </c>
-      <c r="B2" s="53">
-        <v>5</v>
+      <c r="B2">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="109">
+      <c r="A3">
         <v>33</v>
       </c>
-      <c r="B3" s="53">
-        <v>5</v>
+      <c r="B3">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="109">
+      <c r="A4">
         <v>48</v>
       </c>
-      <c r="B4" s="53">
-        <v>17</v>
+      <c r="B4">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="109">
+      <c r="A5">
         <v>49</v>
       </c>
-      <c r="B5" s="53">
-        <v>17</v>
+      <c r="B5">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="109">
+      <c r="A6">
         <v>117</v>
       </c>
-      <c r="B6" s="53">
-        <v>17</v>
+      <c r="B6">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="109">
+      <c r="A7">
         <v>118</v>
       </c>
-      <c r="B7" s="53">
-        <v>17</v>
+      <c r="B7">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="109">
+      <c r="A8">
         <v>123</v>
       </c>
-      <c r="B8" s="53">
-        <v>12</v>
+      <c r="B8">
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="109">
+      <c r="A9">
         <v>124</v>
       </c>
-      <c r="B9" s="53">
-        <v>12</v>
+      <c r="B9">
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="109">
+      <c r="A10">
         <v>133</v>
       </c>
-      <c r="B10" s="53">
-        <v>20</v>
+      <c r="B10">
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="109">
+      <c r="A11">
         <v>134</v>
       </c>
-      <c r="B11" s="53">
-        <v>20</v>
+      <c r="B11">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="109">
+      <c r="A12">
         <v>155</v>
       </c>
-      <c r="B12" s="53">
-        <v>16</v>
+      <c r="B12">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="109">
+      <c r="A13">
         <v>156</v>
       </c>
-      <c r="B13" s="53">
-        <v>16</v>
+      <c r="B13">
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="109">
+      <c r="A14">
         <v>171</v>
       </c>
-      <c r="B14" s="53">
-        <v>17</v>
+      <c r="B14">
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="109">
+      <c r="A15">
         <v>172</v>
       </c>
-      <c r="B15" s="53">
-        <v>17</v>
+      <c r="B15">
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="53">
+      <c r="A16">
         <v>181</v>
       </c>
-      <c r="B16" s="53">
-        <v>16</v>
+      <c r="B16">
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="53">
+      <c r="A17">
         <v>182</v>
       </c>
-      <c r="B17" s="53">
-        <v>16</v>
+      <c r="B17">
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="53">
+      <c r="A18">
         <v>185</v>
       </c>
-      <c r="B18" s="53">
-        <v>16</v>
+      <c r="B18">
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="53">
+      <c r="A19">
         <v>186</v>
       </c>
-      <c r="B19" s="53">
-        <v>16</v>
+      <c r="B19">
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="53">
+      <c r="A20">
         <v>201</v>
       </c>
-      <c r="B20" s="53">
-        <v>16</v>
+      <c r="B20">
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="53">
+      <c r="A21">
         <v>202</v>
       </c>
-      <c r="B21" s="53">
-        <v>16</v>
+      <c r="B21">
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="53">
+      <c r="A22">
         <v>203</v>
       </c>
-      <c r="B22" s="53">
-        <v>17</v>
+      <c r="B22">
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="53">
+      <c r="A23">
         <v>204</v>
       </c>
-      <c r="B23" s="53">
-        <v>17</v>
+      <c r="B23">
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="53">
+      <c r="A24">
         <v>207</v>
       </c>
-      <c r="B24" s="53">
-        <v>16</v>
+      <c r="B24">
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="53">
+      <c r="A25">
         <v>208</v>
       </c>
-      <c r="B25" s="53">
-        <v>16</v>
+      <c r="B25">
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="109">
-        <v>105</v>
-      </c>
-      <c r="B26" s="53">
-        <v>1</v>
-      </c>
+      <c r="A26" s="109"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="109">
-        <v>106</v>
-      </c>
-      <c r="B27" s="53">
-        <v>1</v>
-      </c>
+      <c r="A27" s="109"/>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="109">
-        <v>119</v>
-      </c>
-      <c r="B28" s="53">
-        <v>1</v>
-      </c>
+      <c r="A28" s="109"/>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="109">
-        <v>120</v>
-      </c>
-      <c r="B29" s="53">
-        <v>1</v>
-      </c>
+      <c r="A29" s="109"/>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="109">
-        <v>121</v>
-      </c>
-      <c r="B30" s="53">
-        <v>1</v>
-      </c>
+      <c r="A30" s="109"/>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="109">
-        <v>122</v>
-      </c>
-      <c r="B31" s="53">
-        <v>1</v>
-      </c>
+      <c r="A31" s="109"/>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="109">
-        <v>125</v>
-      </c>
-      <c r="B32" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="109">
-        <v>126</v>
-      </c>
-      <c r="B33" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="109">
-        <v>137</v>
-      </c>
-      <c r="B34" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="109">
-        <v>138</v>
-      </c>
-      <c r="B35" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="109">
-        <v>141</v>
-      </c>
-      <c r="B36" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="109">
-        <v>142</v>
-      </c>
-      <c r="B37" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="109">
-        <v>143</v>
-      </c>
-      <c r="B38" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="109">
-        <v>144</v>
-      </c>
-      <c r="B39" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="109">
-        <v>147</v>
-      </c>
-      <c r="B40" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="109">
-        <v>148</v>
-      </c>
-      <c r="B41" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="109">
-        <v>151</v>
-      </c>
-      <c r="B42" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="109">
-        <v>152</v>
-      </c>
-      <c r="B43" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="109">
-        <v>153</v>
-      </c>
-      <c r="B44" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="109">
-        <v>154</v>
-      </c>
-      <c r="B45" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="109">
-        <v>163</v>
-      </c>
-      <c r="B46" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="109">
-        <v>164</v>
-      </c>
-      <c r="B47" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="109">
-        <v>165</v>
-      </c>
-      <c r="B48" s="53">
-        <v>1</v>
-      </c>
+      <c r="A32" s="109"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="109"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="109"/>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="109"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="109"/>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="109"/>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="109"/>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="109"/>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="109"/>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="109"/>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="109"/>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="109"/>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="109"/>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="109"/>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="109"/>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="109"/>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="109"/>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="109">
-        <v>166</v>
-      </c>
-      <c r="B49" s="53">
-        <v>1</v>
-      </c>
+      <c r="A49" s="109"/>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="109">
-        <v>179</v>
-      </c>
-      <c r="B50" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="53">
-        <v>180</v>
-      </c>
-      <c r="B51" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="53">
-        <v>183</v>
-      </c>
-      <c r="B52" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="53">
-        <v>184</v>
-      </c>
-      <c r="B53" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="53">
-        <v>187</v>
-      </c>
-      <c r="B54" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="53">
-        <v>188</v>
-      </c>
-      <c r="B55" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="53">
-        <v>191</v>
-      </c>
-      <c r="B56" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="53">
-        <v>192</v>
-      </c>
-      <c r="B57" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="53">
-        <v>193</v>
-      </c>
-      <c r="B58" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="53">
-        <v>194</v>
-      </c>
-      <c r="B59" s="53">
-        <v>1</v>
-      </c>
+      <c r="A50" s="109"/>
     </row>
     <row r="60" spans="1:2" s="110" customFormat="1">
-      <c r="A60" s="53">
-        <v>205</v>
-      </c>
-      <c r="B60" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="53">
-        <v>206</v>
-      </c>
-      <c r="B61" s="53">
-        <v>1</v>
-      </c>
+      <c r="A60" s="53"/>
+      <c r="B60" s="53"/>
     </row>
     <row r="62" spans="1:2" s="111" customFormat="1"/>
   </sheetData>

</xml_diff>

<commit_message>
all tests pass, fixtures updated
</commit_message>
<xml_diff>
--- a/tests/_dummy_data.xlsx
+++ b/tests/_dummy_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0C85DA-0233-4443-8143-3E3DB2BDC991}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1409A7-334F-4DFF-87BF-3B495CF5B76E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -1609,7 +1609,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1915,9 +1915,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2321,8 +2318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DU51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AW3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="BE11" sqref="BE11"/>
@@ -2417,106 +2414,106 @@
     <row r="1" spans="1:125" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="100"/>
       <c r="C1" s="16"/>
-      <c r="D1" s="112" t="s">
+      <c r="D1" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="112"/>
-      <c r="G1" s="119" t="s">
+      <c r="E1" s="111"/>
+      <c r="G1" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
-      <c r="K1" s="121" t="s">
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
+      <c r="K1" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="122"/>
-      <c r="M1" s="122"/>
-      <c r="N1" s="122"/>
-      <c r="O1" s="123"/>
-      <c r="S1" s="113"/>
-      <c r="T1" s="113"/>
-      <c r="U1" s="113"/>
-      <c r="V1" s="113"/>
-      <c r="W1" s="113"/>
-      <c r="X1" s="113"/>
-      <c r="Y1" s="113"/>
-      <c r="Z1" s="113"/>
-      <c r="AA1" s="113"/>
-      <c r="AB1" s="113"/>
-      <c r="AC1" s="113"/>
-      <c r="AD1" s="113"/>
-      <c r="AE1" s="113"/>
-      <c r="AF1" s="113"/>
-      <c r="AG1" s="113"/>
-      <c r="AH1" s="113"/>
-      <c r="AI1" s="113"/>
-      <c r="AJ1" s="113"/>
-      <c r="AK1" s="113"/>
+      <c r="L1" s="121"/>
+      <c r="M1" s="121"/>
+      <c r="N1" s="121"/>
+      <c r="O1" s="122"/>
+      <c r="S1" s="112"/>
+      <c r="T1" s="112"/>
+      <c r="U1" s="112"/>
+      <c r="V1" s="112"/>
+      <c r="W1" s="112"/>
+      <c r="X1" s="112"/>
+      <c r="Y1" s="112"/>
+      <c r="Z1" s="112"/>
+      <c r="AA1" s="112"/>
+      <c r="AB1" s="112"/>
+      <c r="AC1" s="112"/>
+      <c r="AD1" s="112"/>
+      <c r="AE1" s="112"/>
+      <c r="AF1" s="112"/>
+      <c r="AG1" s="112"/>
+      <c r="AH1" s="112"/>
+      <c r="AI1" s="112"/>
+      <c r="AJ1" s="112"/>
+      <c r="AK1" s="112"/>
       <c r="AM1" s="99"/>
-      <c r="AN1" s="114" t="s">
+      <c r="AN1" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="AO1" s="113"/>
-      <c r="AP1" s="113"/>
-      <c r="AQ1" s="113"/>
-      <c r="AR1" s="113"/>
-      <c r="AS1" s="113"/>
-      <c r="AT1" s="113"/>
-      <c r="AU1" s="113"/>
-      <c r="AV1" s="113"/>
-      <c r="AW1" s="113"/>
-      <c r="AX1" s="113"/>
-      <c r="AY1" s="113"/>
-      <c r="AZ1" s="113"/>
-      <c r="BA1" s="113"/>
-      <c r="BB1" s="113"/>
-      <c r="BC1" s="113"/>
-      <c r="BD1" s="113"/>
-      <c r="BE1" s="113"/>
-      <c r="BF1" s="113"/>
-      <c r="BG1" s="113"/>
-      <c r="BH1" s="113"/>
-      <c r="BI1" s="113"/>
-      <c r="BJ1" s="113"/>
-      <c r="BK1" s="113"/>
-      <c r="BL1" s="113"/>
-      <c r="BM1" s="113"/>
-      <c r="BN1" s="113"/>
-      <c r="BO1" s="113"/>
-      <c r="BP1" s="113"/>
-      <c r="BR1" s="116"/>
-      <c r="BS1" s="117"/>
-      <c r="BT1" s="117"/>
-      <c r="BU1" s="117"/>
-      <c r="BV1" s="117"/>
-      <c r="BW1" s="118"/>
+      <c r="AO1" s="112"/>
+      <c r="AP1" s="112"/>
+      <c r="AQ1" s="112"/>
+      <c r="AR1" s="112"/>
+      <c r="AS1" s="112"/>
+      <c r="AT1" s="112"/>
+      <c r="AU1" s="112"/>
+      <c r="AV1" s="112"/>
+      <c r="AW1" s="112"/>
+      <c r="AX1" s="112"/>
+      <c r="AY1" s="112"/>
+      <c r="AZ1" s="112"/>
+      <c r="BA1" s="112"/>
+      <c r="BB1" s="112"/>
+      <c r="BC1" s="112"/>
+      <c r="BD1" s="112"/>
+      <c r="BE1" s="112"/>
+      <c r="BF1" s="112"/>
+      <c r="BG1" s="112"/>
+      <c r="BH1" s="112"/>
+      <c r="BI1" s="112"/>
+      <c r="BJ1" s="112"/>
+      <c r="BK1" s="112"/>
+      <c r="BL1" s="112"/>
+      <c r="BM1" s="112"/>
+      <c r="BN1" s="112"/>
+      <c r="BO1" s="112"/>
+      <c r="BP1" s="112"/>
+      <c r="BR1" s="115"/>
+      <c r="BS1" s="116"/>
+      <c r="BT1" s="116"/>
+      <c r="BU1" s="116"/>
+      <c r="BV1" s="116"/>
+      <c r="BW1" s="117"/>
       <c r="BX1" s="102"/>
-      <c r="BZ1" s="113"/>
-      <c r="CA1" s="113"/>
-      <c r="CB1" s="113"/>
-      <c r="CC1" s="113"/>
-      <c r="CD1" s="113"/>
-      <c r="CE1" s="113"/>
-      <c r="CF1" s="113"/>
-      <c r="CG1" s="115"/>
-      <c r="CH1" s="114" t="s">
+      <c r="BZ1" s="112"/>
+      <c r="CA1" s="112"/>
+      <c r="CB1" s="112"/>
+      <c r="CC1" s="112"/>
+      <c r="CD1" s="112"/>
+      <c r="CE1" s="112"/>
+      <c r="CF1" s="112"/>
+      <c r="CG1" s="114"/>
+      <c r="CH1" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="CI1" s="113"/>
-      <c r="CJ1" s="113"/>
-      <c r="CK1" s="113"/>
-      <c r="CL1" s="113"/>
-      <c r="CM1" s="115"/>
+      <c r="CI1" s="112"/>
+      <c r="CJ1" s="112"/>
+      <c r="CK1" s="112"/>
+      <c r="CL1" s="112"/>
+      <c r="CM1" s="114"/>
       <c r="CO1" s="65"/>
-      <c r="CP1" s="113" t="s">
+      <c r="CP1" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="CQ1" s="113"/>
-      <c r="CR1" s="113"/>
-      <c r="CS1" s="113"/>
-      <c r="CT1" s="113"/>
-      <c r="CU1" s="113"/>
-      <c r="CV1" s="113"/>
+      <c r="CQ1" s="112"/>
+      <c r="CR1" s="112"/>
+      <c r="CS1" s="112"/>
+      <c r="CT1" s="112"/>
+      <c r="CU1" s="112"/>
+      <c r="CV1" s="112"/>
       <c r="CX1" s="95"/>
       <c r="CY1" s="95"/>
       <c r="CZ1" s="95"/>
@@ -3629,7 +3626,7 @@
       <c r="DU22" s="33"/>
     </row>
     <row r="23" spans="1:125" ht="30">
-      <c r="A23" s="126" t="s">
+      <c r="A23" s="125" t="s">
         <v>349</v>
       </c>
       <c r="B23" s="32">
@@ -4508,12 +4505,12 @@
     <row r="1" spans="1:8">
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="124" t="s">
+      <c r="E1" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="124"/>
-      <c r="G1" s="124"/>
-      <c r="H1" s="124"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
     </row>
     <row r="2" spans="1:8" ht="45">
       <c r="C2" s="74" t="s">
@@ -4812,11 +4809,11 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="C1" s="2"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="115"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="114"/>
       <c r="I1" s="101"/>
       <c r="J1" s="88"/>
     </row>
@@ -5003,15 +5000,15 @@
     <row r="1" spans="1:11" ht="26.25">
       <c r="C1" s="2"/>
       <c r="D1" s="65"/>
-      <c r="E1" s="125" t="s">
+      <c r="E1" s="124" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="125"/>
-      <c r="I1" s="125"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
+      <c r="I1" s="124"/>
+      <c r="J1" s="124"/>
+      <c r="K1" s="124"/>
     </row>
     <row r="2" spans="1:11" ht="30">
       <c r="C2" s="75" t="s">
@@ -5453,7 +5450,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="75">
-      <c r="A3" s="126" t="s">
+      <c r="A3" s="125" t="s">
         <v>349</v>
       </c>
       <c r="B3" s="32">
@@ -6340,8 +6337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -6393,244 +6390,453 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B6">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="B7">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="B11">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>171</v>
+        <v>123</v>
       </c>
       <c r="B14">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
-        <v>172</v>
+        <v>124</v>
       </c>
       <c r="B15">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16">
-        <v>181</v>
+        <v>125</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>182</v>
+        <v>126</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>185</v>
+        <v>133</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>186</v>
+        <v>134</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>201</v>
+        <v>137</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>202</v>
+        <v>138</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>203</v>
+        <v>141</v>
       </c>
       <c r="B22">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
-        <v>204</v>
+        <v>142</v>
       </c>
       <c r="B23">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24">
-        <v>207</v>
+        <v>143</v>
       </c>
       <c r="B24">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25">
+        <v>144</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26">
+        <v>147</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27">
+        <v>148</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28">
+        <v>151</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29">
+        <v>152</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30">
+        <v>153</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31">
+        <v>154</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32">
+        <v>155</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33">
+        <v>156</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34">
+        <v>163</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35">
+        <v>164</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36">
+        <v>165</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37">
+        <v>166</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38">
+        <v>171</v>
+      </c>
+      <c r="B38">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39">
+        <v>172</v>
+      </c>
+      <c r="B39">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40">
+        <v>179</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41">
+        <v>180</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42">
+        <v>181</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43">
+        <v>182</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44">
+        <v>183</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45">
+        <v>184</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46">
+        <v>185</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47">
+        <v>186</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48">
+        <v>187</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49">
+        <v>188</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50">
+        <v>191</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51">
+        <v>192</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52">
+        <v>193</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53">
+        <v>194</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54">
+        <v>201</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55">
+        <v>202</v>
+      </c>
+      <c r="B55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56">
+        <v>203</v>
+      </c>
+      <c r="B56">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57">
+        <v>204</v>
+      </c>
+      <c r="B57">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58">
+        <v>205</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59">
+        <v>206</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" s="109" customFormat="1">
+      <c r="A60">
+        <v>207</v>
+      </c>
+      <c r="B60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61">
         <v>208</v>
       </c>
-      <c r="B25">
+      <c r="B61">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="109"/>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="109"/>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="109"/>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="109"/>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="109"/>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="109"/>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="109"/>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="109"/>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="109"/>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="109"/>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="109"/>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="109"/>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="109"/>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="109"/>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="109"/>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="109"/>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="109"/>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="109"/>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="109"/>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="109"/>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="109"/>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="109"/>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="109"/>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="109"/>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="109"/>
-    </row>
-    <row r="60" spans="1:2" s="110" customFormat="1">
-      <c r="A60" s="53"/>
-      <c r="B60" s="53"/>
-    </row>
-    <row r="62" spans="1:2" s="111" customFormat="1"/>
+    <row r="62" spans="1:2" s="110" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9806,24 +10012,24 @@
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1">
       <c r="D1" s="73"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
-      <c r="M1" s="113"/>
-      <c r="N1" s="113"/>
-      <c r="O1" s="113"/>
-      <c r="P1" s="113"/>
-      <c r="Q1" s="113"/>
-      <c r="R1" s="113"/>
-      <c r="S1" s="113"/>
-      <c r="T1" s="113"/>
-      <c r="U1" s="113"/>
-      <c r="V1" s="113"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
+      <c r="O1" s="112"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="112"/>
+      <c r="R1" s="112"/>
+      <c r="S1" s="112"/>
+      <c r="T1" s="112"/>
+      <c r="U1" s="112"/>
+      <c r="V1" s="112"/>
     </row>
     <row r="2" spans="1:23" ht="96" customHeight="1">
       <c r="A2" s="42"/>
@@ -10785,37 +10991,37 @@
     <row r="1" spans="1:33" ht="15" customHeight="1">
       <c r="A1" s="42"/>
       <c r="B1" s="43"/>
-      <c r="E1" s="114" t="s">
+      <c r="E1" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
-      <c r="M1" s="113"/>
-      <c r="N1" s="113"/>
-      <c r="O1" s="113"/>
-      <c r="P1" s="113"/>
-      <c r="Q1" s="113"/>
-      <c r="R1" s="113"/>
-      <c r="S1" s="113"/>
-      <c r="T1" s="113"/>
-      <c r="U1" s="113"/>
-      <c r="V1" s="113"/>
-      <c r="W1" s="113"/>
-      <c r="X1" s="113"/>
-      <c r="Y1" s="113"/>
-      <c r="Z1" s="113"/>
-      <c r="AA1" s="113"/>
-      <c r="AB1" s="113"/>
-      <c r="AC1" s="113"/>
-      <c r="AD1" s="113"/>
-      <c r="AE1" s="113"/>
-      <c r="AF1" s="113"/>
-      <c r="AG1" s="113"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
+      <c r="O1" s="112"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="112"/>
+      <c r="R1" s="112"/>
+      <c r="S1" s="112"/>
+      <c r="T1" s="112"/>
+      <c r="U1" s="112"/>
+      <c r="V1" s="112"/>
+      <c r="W1" s="112"/>
+      <c r="X1" s="112"/>
+      <c r="Y1" s="112"/>
+      <c r="Z1" s="112"/>
+      <c r="AA1" s="112"/>
+      <c r="AB1" s="112"/>
+      <c r="AC1" s="112"/>
+      <c r="AD1" s="112"/>
+      <c r="AE1" s="112"/>
+      <c r="AF1" s="112"/>
+      <c r="AG1" s="112"/>
     </row>
     <row r="2" spans="1:33" ht="144" customHeight="1">
       <c r="C2" s="73" t="s">

</xml_diff>

<commit_message>
dummy data for testing tonic vs asymmetric tonic
</commit_message>
<xml_diff>
--- a/tests/_dummy_data.xlsx
+++ b/tests/_dummy_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1409A7-334F-4DFF-87BF-3B495CF5B76E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06E38C0-1D0E-416B-9844-88EF7336BDE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="364">
   <si>
     <t xml:space="preserve">Semiology </t>
   </si>
@@ -1115,6 +1115,33 @@
   </si>
   <si>
     <t>IFG FL</t>
+  </si>
+  <si>
+    <t>tonic vs asymmetric tonic 1</t>
+  </si>
+  <si>
+    <t>tonic vs asymmetric tonic 2</t>
+  </si>
+  <si>
+    <t>asymmetric tonic</t>
+  </si>
+  <si>
+    <t>tonic</t>
+  </si>
+  <si>
+    <t>Asymmetric Tonic</t>
+  </si>
+  <si>
+    <t>SMA</t>
+  </si>
+  <si>
+    <t>precentral gyrus</t>
+  </si>
+  <si>
+    <t>y+CX5:DG5</t>
+  </si>
+  <si>
+    <t>Romagnoli et al as above in adult</t>
   </si>
 </sst>
 </file>
@@ -1923,6 +1950,9 @@
     <xf numFmtId="0" fontId="21" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1964,9 +1994,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2316,13 +2343,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DU51"/>
+  <dimension ref="A1:DU52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BE11" sqref="BE11"/>
+      <selection pane="bottomRight" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2414,106 +2441,106 @@
     <row r="1" spans="1:125" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="100"/>
       <c r="C1" s="16"/>
-      <c r="D1" s="111" t="s">
+      <c r="D1" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="111"/>
-      <c r="G1" s="118" t="s">
+      <c r="E1" s="112"/>
+      <c r="G1" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="119"/>
-      <c r="I1" s="119"/>
-      <c r="K1" s="120" t="s">
+      <c r="H1" s="120"/>
+      <c r="I1" s="120"/>
+      <c r="K1" s="121" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="121"/>
-      <c r="M1" s="121"/>
-      <c r="N1" s="121"/>
-      <c r="O1" s="122"/>
-      <c r="S1" s="112"/>
-      <c r="T1" s="112"/>
-      <c r="U1" s="112"/>
-      <c r="V1" s="112"/>
-      <c r="W1" s="112"/>
-      <c r="X1" s="112"/>
-      <c r="Y1" s="112"/>
-      <c r="Z1" s="112"/>
-      <c r="AA1" s="112"/>
-      <c r="AB1" s="112"/>
-      <c r="AC1" s="112"/>
-      <c r="AD1" s="112"/>
-      <c r="AE1" s="112"/>
-      <c r="AF1" s="112"/>
-      <c r="AG1" s="112"/>
-      <c r="AH1" s="112"/>
-      <c r="AI1" s="112"/>
-      <c r="AJ1" s="112"/>
-      <c r="AK1" s="112"/>
+      <c r="L1" s="122"/>
+      <c r="M1" s="122"/>
+      <c r="N1" s="122"/>
+      <c r="O1" s="123"/>
+      <c r="S1" s="113"/>
+      <c r="T1" s="113"/>
+      <c r="U1" s="113"/>
+      <c r="V1" s="113"/>
+      <c r="W1" s="113"/>
+      <c r="X1" s="113"/>
+      <c r="Y1" s="113"/>
+      <c r="Z1" s="113"/>
+      <c r="AA1" s="113"/>
+      <c r="AB1" s="113"/>
+      <c r="AC1" s="113"/>
+      <c r="AD1" s="113"/>
+      <c r="AE1" s="113"/>
+      <c r="AF1" s="113"/>
+      <c r="AG1" s="113"/>
+      <c r="AH1" s="113"/>
+      <c r="AI1" s="113"/>
+      <c r="AJ1" s="113"/>
+      <c r="AK1" s="113"/>
       <c r="AM1" s="99"/>
-      <c r="AN1" s="113" t="s">
+      <c r="AN1" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="AO1" s="112"/>
-      <c r="AP1" s="112"/>
-      <c r="AQ1" s="112"/>
-      <c r="AR1" s="112"/>
-      <c r="AS1" s="112"/>
-      <c r="AT1" s="112"/>
-      <c r="AU1" s="112"/>
-      <c r="AV1" s="112"/>
-      <c r="AW1" s="112"/>
-      <c r="AX1" s="112"/>
-      <c r="AY1" s="112"/>
-      <c r="AZ1" s="112"/>
-      <c r="BA1" s="112"/>
-      <c r="BB1" s="112"/>
-      <c r="BC1" s="112"/>
-      <c r="BD1" s="112"/>
-      <c r="BE1" s="112"/>
-      <c r="BF1" s="112"/>
-      <c r="BG1" s="112"/>
-      <c r="BH1" s="112"/>
-      <c r="BI1" s="112"/>
-      <c r="BJ1" s="112"/>
-      <c r="BK1" s="112"/>
-      <c r="BL1" s="112"/>
-      <c r="BM1" s="112"/>
-      <c r="BN1" s="112"/>
-      <c r="BO1" s="112"/>
-      <c r="BP1" s="112"/>
-      <c r="BR1" s="115"/>
-      <c r="BS1" s="116"/>
-      <c r="BT1" s="116"/>
-      <c r="BU1" s="116"/>
-      <c r="BV1" s="116"/>
-      <c r="BW1" s="117"/>
+      <c r="AO1" s="113"/>
+      <c r="AP1" s="113"/>
+      <c r="AQ1" s="113"/>
+      <c r="AR1" s="113"/>
+      <c r="AS1" s="113"/>
+      <c r="AT1" s="113"/>
+      <c r="AU1" s="113"/>
+      <c r="AV1" s="113"/>
+      <c r="AW1" s="113"/>
+      <c r="AX1" s="113"/>
+      <c r="AY1" s="113"/>
+      <c r="AZ1" s="113"/>
+      <c r="BA1" s="113"/>
+      <c r="BB1" s="113"/>
+      <c r="BC1" s="113"/>
+      <c r="BD1" s="113"/>
+      <c r="BE1" s="113"/>
+      <c r="BF1" s="113"/>
+      <c r="BG1" s="113"/>
+      <c r="BH1" s="113"/>
+      <c r="BI1" s="113"/>
+      <c r="BJ1" s="113"/>
+      <c r="BK1" s="113"/>
+      <c r="BL1" s="113"/>
+      <c r="BM1" s="113"/>
+      <c r="BN1" s="113"/>
+      <c r="BO1" s="113"/>
+      <c r="BP1" s="113"/>
+      <c r="BR1" s="116"/>
+      <c r="BS1" s="117"/>
+      <c r="BT1" s="117"/>
+      <c r="BU1" s="117"/>
+      <c r="BV1" s="117"/>
+      <c r="BW1" s="118"/>
       <c r="BX1" s="102"/>
-      <c r="BZ1" s="112"/>
-      <c r="CA1" s="112"/>
-      <c r="CB1" s="112"/>
-      <c r="CC1" s="112"/>
-      <c r="CD1" s="112"/>
-      <c r="CE1" s="112"/>
-      <c r="CF1" s="112"/>
-      <c r="CG1" s="114"/>
-      <c r="CH1" s="113" t="s">
+      <c r="BZ1" s="113"/>
+      <c r="CA1" s="113"/>
+      <c r="CB1" s="113"/>
+      <c r="CC1" s="113"/>
+      <c r="CD1" s="113"/>
+      <c r="CE1" s="113"/>
+      <c r="CF1" s="113"/>
+      <c r="CG1" s="115"/>
+      <c r="CH1" s="114" t="s">
         <v>4</v>
       </c>
-      <c r="CI1" s="112"/>
-      <c r="CJ1" s="112"/>
-      <c r="CK1" s="112"/>
-      <c r="CL1" s="112"/>
-      <c r="CM1" s="114"/>
+      <c r="CI1" s="113"/>
+      <c r="CJ1" s="113"/>
+      <c r="CK1" s="113"/>
+      <c r="CL1" s="113"/>
+      <c r="CM1" s="115"/>
       <c r="CO1" s="65"/>
-      <c r="CP1" s="112" t="s">
+      <c r="CP1" s="113" t="s">
         <v>5</v>
       </c>
-      <c r="CQ1" s="112"/>
-      <c r="CR1" s="112"/>
-      <c r="CS1" s="112"/>
-      <c r="CT1" s="112"/>
-      <c r="CU1" s="112"/>
-      <c r="CV1" s="112"/>
+      <c r="CQ1" s="113"/>
+      <c r="CR1" s="113"/>
+      <c r="CS1" s="113"/>
+      <c r="CT1" s="113"/>
+      <c r="CU1" s="113"/>
+      <c r="CV1" s="113"/>
       <c r="CX1" s="95"/>
       <c r="CY1" s="95"/>
       <c r="CZ1" s="95"/>
@@ -2964,173 +2991,197 @@
       <c r="DT4" s="33"/>
       <c r="DU4" s="33"/>
     </row>
-    <row r="5" spans="1:125" ht="30">
-      <c r="A5" s="32" t="s">
-        <v>303</v>
-      </c>
-      <c r="B5" s="32">
+    <row r="7" spans="1:125" s="33" customFormat="1">
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="5"/>
+      <c r="AF7" s="5"/>
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="5"/>
+      <c r="AI7" s="5"/>
+      <c r="AJ7" s="5"/>
+      <c r="AK7" s="5"/>
+      <c r="AL7" s="5"/>
+      <c r="AM7" s="5"/>
+      <c r="AN7" s="5"/>
+      <c r="AO7" s="5"/>
+      <c r="AP7" s="5"/>
+      <c r="AQ7" s="5"/>
+      <c r="AR7" s="5"/>
+      <c r="AS7" s="5"/>
+      <c r="AT7" s="5"/>
+      <c r="AU7" s="5"/>
+      <c r="AV7" s="5"/>
+      <c r="AW7" s="5"/>
+      <c r="AX7" s="5"/>
+      <c r="AY7" s="5"/>
+      <c r="AZ7" s="5"/>
+      <c r="BA7" s="5"/>
+      <c r="BB7" s="5"/>
+      <c r="BC7" s="5"/>
+      <c r="BD7" s="5"/>
+      <c r="BE7" s="5"/>
+      <c r="BF7" s="5"/>
+      <c r="BG7" s="5"/>
+      <c r="BH7" s="5"/>
+      <c r="BI7" s="5"/>
+      <c r="BJ7" s="5"/>
+      <c r="BK7" s="5"/>
+      <c r="BL7" s="5"/>
+      <c r="BM7" s="5"/>
+      <c r="BN7" s="5"/>
+      <c r="BO7" s="5"/>
+      <c r="BP7" s="5"/>
+      <c r="BQ7" s="5"/>
+      <c r="BR7" s="5"/>
+      <c r="BS7" s="5"/>
+      <c r="BT7" s="5"/>
+      <c r="BU7" s="5"/>
+      <c r="BV7" s="5"/>
+      <c r="BW7" s="5"/>
+      <c r="BX7" s="5"/>
+      <c r="BY7" s="5"/>
+      <c r="BZ7" s="5"/>
+      <c r="CA7" s="5"/>
+      <c r="CB7" s="5"/>
+      <c r="CC7" s="5"/>
+      <c r="CD7" s="5"/>
+      <c r="CE7" s="5"/>
+      <c r="CF7" s="5"/>
+      <c r="CG7" s="5"/>
+      <c r="CH7" s="5"/>
+      <c r="CI7" s="5"/>
+      <c r="CJ7" s="5"/>
+      <c r="CK7" s="5"/>
+      <c r="CL7" s="5"/>
+      <c r="CM7" s="5"/>
+      <c r="CN7" s="5"/>
+      <c r="CO7" s="5"/>
+      <c r="CP7" s="5"/>
+      <c r="CQ7" s="5"/>
+      <c r="CR7" s="5"/>
+      <c r="CS7" s="5"/>
+      <c r="CT7" s="5"/>
+      <c r="CU7" s="5"/>
+      <c r="CV7" s="5"/>
+      <c r="CW7" s="5"/>
+      <c r="CX7" s="5"/>
+      <c r="CY7" s="5"/>
+      <c r="CZ7" s="5"/>
+      <c r="DA7" s="5"/>
+      <c r="DB7" s="6"/>
+      <c r="DC7" s="6"/>
+      <c r="DD7" s="5"/>
+      <c r="DE7" s="5"/>
+      <c r="DF7" s="5"/>
+      <c r="DG7" s="5"/>
+      <c r="DH7" s="5"/>
+      <c r="DI7" s="5"/>
+      <c r="DJ7" s="5"/>
+      <c r="DK7" s="5"/>
+      <c r="DL7" s="5"/>
+      <c r="DM7" s="5"/>
+      <c r="DN7" s="5"/>
+      <c r="DO7" s="5"/>
+    </row>
+    <row r="8" spans="1:125" ht="30">
+      <c r="A8" s="32" t="s">
+        <v>305</v>
+      </c>
+      <c r="B8" s="32">
+        <v>10</v>
+      </c>
+      <c r="C8" s="32">
+        <v>10</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>306</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>307</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>309</v>
+      </c>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32" t="s">
+        <v>308</v>
+      </c>
+      <c r="I8" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="M8" s="5">
+        <v>10</v>
+      </c>
+      <c r="P8" s="5">
+        <v>10</v>
+      </c>
+      <c r="Q8" s="31" t="s">
+        <v>310</v>
+      </c>
+      <c r="AL8" s="5">
+        <v>10</v>
+      </c>
+      <c r="AN8" s="5">
+        <v>5</v>
+      </c>
+      <c r="AV8" s="5">
+        <v>5</v>
+      </c>
+      <c r="AW8" s="5">
         <v>1</v>
       </c>
-      <c r="C5" s="32">
-        <v>1</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>299</v>
-      </c>
-      <c r="E5" s="33" t="s">
-        <v>300</v>
-      </c>
-      <c r="F5" s="32" t="s">
-        <v>301</v>
-      </c>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32" t="s">
+      <c r="BQ8" s="5">
+        <v>2</v>
+      </c>
+      <c r="BS8" s="5">
+        <v>2</v>
+      </c>
+      <c r="DA8" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="DB8" s="6">
+        <v>10</v>
+      </c>
+      <c r="DC8" s="6">
+        <v>0</v>
+      </c>
+      <c r="DD8" s="5">
+        <v>0</v>
+      </c>
+      <c r="DE8" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="I5" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="J5" s="5">
-        <v>1</v>
-      </c>
-      <c r="K5" s="5">
-        <v>1</v>
-      </c>
-      <c r="P5" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="31" t="s">
-        <v>302</v>
-      </c>
-      <c r="AL5" s="5">
-        <v>1</v>
-      </c>
-      <c r="AW5" s="5">
-        <v>1</v>
-      </c>
-      <c r="DA5" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="DB5" s="6">
-        <v>1</v>
-      </c>
-      <c r="DC5" s="6">
-        <v>0</v>
-      </c>
-      <c r="DD5" s="5">
-        <v>0</v>
-      </c>
-      <c r="DG5" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="DP5" s="33"/>
-      <c r="DQ5" s="33"/>
-      <c r="DR5" s="33"/>
-      <c r="DS5" s="33"/>
-      <c r="DT5" s="33"/>
-      <c r="DU5" s="33"/>
-    </row>
-    <row r="6" spans="1:125">
-      <c r="A6" s="32"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="DP6" s="33"/>
-      <c r="DQ6" s="33"/>
-      <c r="DR6" s="33"/>
-      <c r="DS6" s="33"/>
-      <c r="DT6" s="33"/>
-      <c r="DU6" s="33"/>
-    </row>
-    <row r="7" spans="1:125" ht="30">
-      <c r="A7" s="32" t="s">
-        <v>305</v>
-      </c>
-      <c r="B7" s="32">
-        <v>10</v>
-      </c>
-      <c r="C7" s="32">
-        <v>10</v>
-      </c>
-      <c r="D7" s="32" t="s">
-        <v>306</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>307</v>
-      </c>
-      <c r="F7" s="32" t="s">
-        <v>309</v>
-      </c>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32" t="s">
-        <v>308</v>
-      </c>
-      <c r="I7" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="M7" s="5">
-        <v>10</v>
-      </c>
-      <c r="P7" s="5">
-        <v>10</v>
-      </c>
-      <c r="Q7" s="31" t="s">
-        <v>310</v>
-      </c>
-      <c r="AL7" s="5">
-        <v>10</v>
-      </c>
-      <c r="AN7" s="5">
-        <v>5</v>
-      </c>
-      <c r="AV7" s="5">
-        <v>5</v>
-      </c>
-      <c r="AW7" s="5">
-        <v>1</v>
-      </c>
-      <c r="BQ7" s="5">
-        <v>2</v>
-      </c>
-      <c r="BS7" s="5">
-        <v>2</v>
-      </c>
-      <c r="DA7" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="DB7" s="6">
-        <v>10</v>
-      </c>
-      <c r="DC7" s="6">
-        <v>0</v>
-      </c>
-      <c r="DD7" s="5">
-        <v>0</v>
-      </c>
-      <c r="DE7" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="DH7" s="5" t="s">
+      <c r="DH8" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="DP7" s="33"/>
-      <c r="DQ7" s="33"/>
-      <c r="DR7" s="33"/>
-      <c r="DS7" s="33"/>
-      <c r="DT7" s="33"/>
-      <c r="DU7" s="33"/>
-    </row>
-    <row r="8" spans="1:125">
-      <c r="A8" s="32"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
       <c r="DP8" s="33"/>
       <c r="DQ8" s="33"/>
       <c r="DR8" s="33"/>
@@ -3139,71 +3190,13 @@
       <c r="DU8" s="33"/>
     </row>
     <row r="9" spans="1:125">
-      <c r="A9" s="32" t="s">
-        <v>311</v>
-      </c>
-      <c r="B9" s="32">
-        <v>10</v>
-      </c>
-      <c r="C9" s="32">
-        <v>10</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>118</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>316</v>
-      </c>
-      <c r="F9" s="32" t="s">
-        <v>295</v>
-      </c>
-      <c r="G9" s="32" t="s">
-        <v>116</v>
-      </c>
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="G9" s="32"/>
       <c r="H9" s="32"/>
       <c r="I9" s="32"/>
-      <c r="J9" s="5">
-        <v>5</v>
-      </c>
-      <c r="N9" s="5">
-        <v>5</v>
-      </c>
-      <c r="P9" s="5">
-        <v>9</v>
-      </c>
-      <c r="Q9" s="31" t="s">
-        <v>315</v>
-      </c>
-      <c r="R9" s="5">
-        <v>9</v>
-      </c>
-      <c r="S9" s="5">
-        <v>5</v>
-      </c>
-      <c r="T9" s="5">
-        <v>4</v>
-      </c>
-      <c r="Z9" s="5">
-        <v>4</v>
-      </c>
-      <c r="AA9" s="5">
-        <v>5</v>
-      </c>
-      <c r="DA9" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="DB9" s="6">
-        <v>10</v>
-      </c>
-      <c r="DC9" s="6">
-        <v>0</v>
-      </c>
-      <c r="DD9" s="5">
-        <v>10</v>
-      </c>
-      <c r="DF9" s="5" t="s">
-        <v>116</v>
-      </c>
       <c r="DP9" s="33"/>
       <c r="DQ9" s="33"/>
       <c r="DR9" s="33"/>
@@ -3212,17 +3205,23 @@
       <c r="DU9" s="33"/>
     </row>
     <row r="10" spans="1:125">
-      <c r="A10" s="17"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
+      <c r="A10" s="32" t="s">
+        <v>311</v>
+      </c>
+      <c r="B10" s="32">
+        <v>10</v>
+      </c>
+      <c r="C10" s="32">
+        <v>10</v>
+      </c>
       <c r="D10" s="32" t="s">
-        <v>312</v>
+        <v>118</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="F10" s="32" t="s">
-        <v>313</v>
+        <v>295</v>
       </c>
       <c r="G10" s="32" t="s">
         <v>116</v>
@@ -3230,25 +3229,46 @@
       <c r="H10" s="32"/>
       <c r="I10" s="32"/>
       <c r="J10" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N10" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P10" s="5">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="Q10" s="31" t="s">
-        <v>314</v>
-      </c>
-      <c r="AL10" s="5">
-        <v>1</v>
-      </c>
-      <c r="BE10" s="5">
-        <v>1</v>
+        <v>315</v>
+      </c>
+      <c r="R10" s="5">
+        <v>9</v>
+      </c>
+      <c r="S10" s="5">
+        <v>5</v>
+      </c>
+      <c r="T10" s="5">
+        <v>4</v>
+      </c>
+      <c r="Z10" s="5">
+        <v>4</v>
+      </c>
+      <c r="AA10" s="5">
+        <v>5</v>
       </c>
       <c r="DA10" s="5" t="s">
         <v>297</v>
+      </c>
+      <c r="DB10" s="6">
+        <v>10</v>
+      </c>
+      <c r="DC10" s="6">
+        <v>0</v>
+      </c>
+      <c r="DD10" s="5">
+        <v>10</v>
+      </c>
+      <c r="DF10" s="5" t="s">
+        <v>116</v>
       </c>
       <c r="DP10" s="33"/>
       <c r="DQ10" s="33"/>
@@ -3258,20 +3278,14 @@
       <c r="DU10" s="33"/>
     </row>
     <row r="11" spans="1:125">
-      <c r="A11" s="32" t="s">
-        <v>352</v>
-      </c>
-      <c r="B11" s="32">
-        <v>1</v>
-      </c>
-      <c r="C11" s="32">
-        <v>1</v>
-      </c>
+      <c r="A11" s="17"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
       <c r="D11" s="32" t="s">
-        <v>353</v>
+        <v>312</v>
       </c>
       <c r="E11" s="33" t="s">
-        <v>118</v>
+        <v>312</v>
       </c>
       <c r="F11" s="32" t="s">
         <v>313</v>
@@ -3281,17 +3295,26 @@
       </c>
       <c r="H11" s="32"/>
       <c r="I11" s="32"/>
+      <c r="J11" s="5">
+        <v>1</v>
+      </c>
+      <c r="N11" s="5">
+        <v>1</v>
+      </c>
       <c r="P11" s="5">
         <v>1</v>
       </c>
       <c r="Q11" s="31" t="s">
-        <v>354</v>
+        <v>314</v>
       </c>
       <c r="AL11" s="5">
         <v>1</v>
       </c>
       <c r="BE11" s="5">
         <v>1</v>
+      </c>
+      <c r="DA11" s="5" t="s">
+        <v>297</v>
       </c>
       <c r="DP11" s="33"/>
       <c r="DQ11" s="33"/>
@@ -3301,13 +3324,41 @@
       <c r="DU11" s="33"/>
     </row>
     <row r="12" spans="1:125">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="G12" s="32"/>
+      <c r="A12" s="32" t="s">
+        <v>352</v>
+      </c>
+      <c r="B12" s="32">
+        <v>1</v>
+      </c>
+      <c r="C12" s="32">
+        <v>1</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>313</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>116</v>
+      </c>
       <c r="H12" s="32"/>
       <c r="I12" s="32"/>
+      <c r="P12" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="31" t="s">
+        <v>354</v>
+      </c>
+      <c r="AL12" s="5">
+        <v>1</v>
+      </c>
+      <c r="BE12" s="5">
+        <v>1</v>
+      </c>
       <c r="DP12" s="33"/>
       <c r="DQ12" s="33"/>
       <c r="DR12" s="33"/>
@@ -3316,53 +3367,13 @@
       <c r="DU12" s="33"/>
     </row>
     <row r="13" spans="1:125">
-      <c r="A13" s="32" t="s">
-        <v>319</v>
-      </c>
-      <c r="B13" s="32">
-        <v>1</v>
-      </c>
-      <c r="C13" s="32">
-        <v>1</v>
-      </c>
-      <c r="D13" s="32" t="s">
-        <v>118</v>
-      </c>
-      <c r="E13" s="33" t="s">
-        <v>317</v>
-      </c>
-      <c r="F13" s="32" t="s">
-        <v>318</v>
-      </c>
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
       <c r="G13" s="32"/>
-      <c r="H13" s="32" t="s">
-        <v>116</v>
-      </c>
+      <c r="H13" s="32"/>
       <c r="I13" s="32"/>
-      <c r="P13" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="R13" s="5">
-        <v>1</v>
-      </c>
-      <c r="DA13" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="DB13" s="6">
-        <v>1</v>
-      </c>
-      <c r="DC13" s="6">
-        <v>0</v>
-      </c>
-      <c r="DD13" s="5">
-        <v>0</v>
-      </c>
-      <c r="DF13" s="5" t="s">
-        <v>116</v>
-      </c>
       <c r="DP13" s="33"/>
       <c r="DQ13" s="33"/>
       <c r="DR13" s="33"/>
@@ -3372,7 +3383,7 @@
     </row>
     <row r="14" spans="1:125">
       <c r="A14" s="32" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B14" s="32">
         <v>1</v>
@@ -3380,11 +3391,11 @@
       <c r="C14" s="32">
         <v>1</v>
       </c>
-      <c r="D14" s="33" t="s">
-        <v>329</v>
+      <c r="D14" s="32" t="s">
+        <v>118</v>
       </c>
       <c r="E14" s="33" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="F14" s="32" t="s">
         <v>318</v>
@@ -3427,7 +3438,7 @@
     </row>
     <row r="15" spans="1:125">
       <c r="A15" s="32" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B15" s="32">
         <v>1</v>
@@ -3435,11 +3446,11 @@
       <c r="C15" s="32">
         <v>1</v>
       </c>
-      <c r="D15" s="32" t="s">
-        <v>322</v>
+      <c r="D15" s="33" t="s">
+        <v>329</v>
       </c>
       <c r="E15" s="33" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="F15" s="32" t="s">
         <v>318</v>
@@ -3481,13 +3492,53 @@
       <c r="DU15" s="33"/>
     </row>
     <row r="16" spans="1:125">
-      <c r="A16" s="32"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
+      <c r="A16" s="32" t="s">
+        <v>321</v>
+      </c>
+      <c r="B16" s="32">
+        <v>1</v>
+      </c>
+      <c r="C16" s="32">
+        <v>1</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>322</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>318</v>
+      </c>
       <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
+      <c r="H16" s="32" t="s">
+        <v>116</v>
+      </c>
       <c r="I16" s="32"/>
+      <c r="P16" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="R16" s="5">
+        <v>1</v>
+      </c>
+      <c r="DA16" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="DB16" s="6">
+        <v>1</v>
+      </c>
+      <c r="DC16" s="6">
+        <v>0</v>
+      </c>
+      <c r="DD16" s="5">
+        <v>0</v>
+      </c>
+      <c r="DF16" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="DP16" s="33"/>
       <c r="DQ16" s="33"/>
       <c r="DR16" s="33"/>
@@ -3571,53 +3622,13 @@
       <c r="DU21" s="33"/>
     </row>
     <row r="22" spans="1:125">
-      <c r="A22" s="17" t="s">
-        <v>340</v>
-      </c>
-      <c r="B22" s="32">
-        <v>10</v>
-      </c>
-      <c r="C22" s="32">
-        <v>10</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>341</v>
-      </c>
-      <c r="E22" s="33" t="s">
-        <v>342</v>
-      </c>
-      <c r="F22" s="32" t="s">
-        <v>343</v>
-      </c>
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
       <c r="G22" s="32"/>
-      <c r="H22" s="32" t="s">
-        <v>116</v>
-      </c>
+      <c r="H22" s="32"/>
       <c r="I22" s="32"/>
-      <c r="M22" s="5">
-        <v>2</v>
-      </c>
-      <c r="P22" s="5">
-        <v>10</v>
-      </c>
-      <c r="Q22" s="31" t="s">
-        <v>344</v>
-      </c>
-      <c r="BQ22" s="5">
-        <v>3</v>
-      </c>
-      <c r="BY22" s="5">
-        <v>4</v>
-      </c>
-      <c r="CN22" s="5">
-        <v>3</v>
-      </c>
-      <c r="DA22" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="DF22" s="5" t="s">
-        <v>116</v>
-      </c>
       <c r="DP22" s="33"/>
       <c r="DQ22" s="33"/>
       <c r="DR22" s="33"/>
@@ -3625,21 +3636,21 @@
       <c r="DT22" s="33"/>
       <c r="DU22" s="33"/>
     </row>
-    <row r="23" spans="1:125" ht="30">
-      <c r="A23" s="125" t="s">
-        <v>349</v>
+    <row r="23" spans="1:125">
+      <c r="A23" s="17" t="s">
+        <v>340</v>
       </c>
       <c r="B23" s="32">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C23" s="32">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="E23" s="33" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="F23" s="32" t="s">
         <v>343</v>
@@ -3649,17 +3660,29 @@
         <v>116</v>
       </c>
       <c r="I23" s="32"/>
+      <c r="M23" s="5">
+        <v>2</v>
+      </c>
       <c r="P23" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="Q23" s="31" t="s">
-        <v>346</v>
-      </c>
-      <c r="R23" s="5">
-        <v>5</v>
-      </c>
-      <c r="AA23" s="5">
-        <v>5</v>
+        <v>344</v>
+      </c>
+      <c r="BQ23" s="5">
+        <v>3</v>
+      </c>
+      <c r="BY23" s="5">
+        <v>4</v>
+      </c>
+      <c r="CN23" s="5">
+        <v>3</v>
+      </c>
+      <c r="DA23" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="DF23" s="5" t="s">
+        <v>116</v>
       </c>
       <c r="DP23" s="33"/>
       <c r="DQ23" s="33"/>
@@ -3668,18 +3691,18 @@
       <c r="DT23" s="33"/>
       <c r="DU23" s="33"/>
     </row>
-    <row r="24" spans="1:125">
-      <c r="A24" s="17" t="s">
-        <v>350</v>
+    <row r="24" spans="1:125" ht="30">
+      <c r="A24" s="111" t="s">
+        <v>349</v>
       </c>
       <c r="B24" s="32">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C24" s="32">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E24" s="33" t="s">
         <v>351</v>
@@ -3693,19 +3716,19 @@
       </c>
       <c r="I24" s="32"/>
       <c r="P24" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q24" s="31" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="R24" s="5">
-        <v>1</v>
-      </c>
-      <c r="AL24" s="5">
-        <v>1</v>
-      </c>
-      <c r="DA24" s="5" t="s">
-        <v>297</v>
+        <v>5</v>
+      </c>
+      <c r="AA24" s="5">
+        <v>5</v>
+      </c>
+      <c r="DF24" s="5" t="s">
+        <v>116</v>
       </c>
       <c r="DP24" s="33"/>
       <c r="DQ24" s="33"/>
@@ -3715,13 +3738,47 @@
       <c r="DU24" s="33"/>
     </row>
     <row r="25" spans="1:125">
-      <c r="A25" s="32"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="17"/>
+      <c r="A25" s="17" t="s">
+        <v>350</v>
+      </c>
+      <c r="B25" s="32">
+        <v>1</v>
+      </c>
+      <c r="C25" s="32">
+        <v>1</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>348</v>
+      </c>
+      <c r="E25" s="33" t="s">
+        <v>351</v>
+      </c>
+      <c r="F25" s="32" t="s">
+        <v>343</v>
+      </c>
       <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
+      <c r="H25" s="32" t="s">
+        <v>116</v>
+      </c>
       <c r="I25" s="32"/>
+      <c r="P25" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="31" t="s">
+        <v>345</v>
+      </c>
+      <c r="R25" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL25" s="5">
+        <v>1</v>
+      </c>
+      <c r="DA25" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="DF25" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="DP25" s="33"/>
       <c r="DQ25" s="33"/>
       <c r="DR25" s="33"/>
@@ -3760,13 +3817,41 @@
       <c r="DU27" s="33"/>
     </row>
     <row r="28" spans="1:125">
-      <c r="A28" s="32"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="17"/>
-      <c r="G28" s="32"/>
+      <c r="A28" s="32" t="s">
+        <v>355</v>
+      </c>
+      <c r="B28" s="32">
+        <v>1</v>
+      </c>
+      <c r="C28" s="32">
+        <v>1</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>357</v>
+      </c>
+      <c r="E28" s="33" t="s">
+        <v>359</v>
+      </c>
+      <c r="G28" s="32" t="s">
+        <v>116</v>
+      </c>
       <c r="H28" s="32"/>
       <c r="I28" s="32"/>
+      <c r="P28" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="31" t="s">
+        <v>360</v>
+      </c>
+      <c r="AL28" s="5">
+        <v>1</v>
+      </c>
+      <c r="BO28" s="5">
+        <v>1</v>
+      </c>
+      <c r="DF28" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="DP28" s="33"/>
       <c r="DQ28" s="33"/>
       <c r="DR28" s="33"/>
@@ -3775,13 +3860,41 @@
       <c r="DU28" s="33"/>
     </row>
     <row r="29" spans="1:125">
-      <c r="A29" s="32"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="17"/>
-      <c r="G29" s="32"/>
+      <c r="A29" s="32" t="s">
+        <v>356</v>
+      </c>
+      <c r="B29" s="32">
+        <v>1</v>
+      </c>
+      <c r="C29" s="32">
+        <v>1</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>358</v>
+      </c>
+      <c r="E29" s="33" t="s">
+        <v>358</v>
+      </c>
+      <c r="G29" s="32" t="s">
+        <v>116</v>
+      </c>
       <c r="H29" s="32"/>
       <c r="I29" s="32"/>
+      <c r="P29" s="5">
+        <v>10</v>
+      </c>
+      <c r="Q29" s="31" t="s">
+        <v>361</v>
+      </c>
+      <c r="AL29" s="5">
+        <v>10</v>
+      </c>
+      <c r="AW29" s="5">
+        <v>10</v>
+      </c>
+      <c r="DF29" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="DP29" s="33"/>
       <c r="DQ29" s="33"/>
       <c r="DR29" s="33"/>
@@ -3789,14 +3902,65 @@
       <c r="DT29" s="33"/>
       <c r="DU29" s="33"/>
     </row>
-    <row r="30" spans="1:125">
-      <c r="A30" s="32"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="17"/>
+    <row r="30" spans="1:125" ht="30">
+      <c r="A30" s="32" t="s">
+        <v>303</v>
+      </c>
+      <c r="B30" s="32">
+        <v>1</v>
+      </c>
+      <c r="C30" s="32">
+        <v>1</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="E30" s="33" t="s">
+        <v>300</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>301</v>
+      </c>
       <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="32"/>
+      <c r="H30" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="I30" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="J30" s="5">
+        <v>1</v>
+      </c>
+      <c r="K30" s="5">
+        <v>1</v>
+      </c>
+      <c r="P30" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="31" t="s">
+        <v>302</v>
+      </c>
+      <c r="AL30" s="5">
+        <v>1</v>
+      </c>
+      <c r="AW30" s="5">
+        <v>1</v>
+      </c>
+      <c r="DA30" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="DB30" s="6">
+        <v>1</v>
+      </c>
+      <c r="DC30" s="6">
+        <v>0</v>
+      </c>
+      <c r="DD30" s="5">
+        <v>0</v>
+      </c>
+      <c r="DG30" s="5" t="s">
+        <v>362</v>
+      </c>
       <c r="DP30" s="33"/>
       <c r="DQ30" s="33"/>
       <c r="DR30" s="33"/>
@@ -3804,20 +3968,164 @@
       <c r="DT30" s="33"/>
       <c r="DU30" s="33"/>
     </row>
-    <row r="31" spans="1:125">
-      <c r="A31" s="32"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="17"/>
+    <row r="31" spans="1:125" s="33" customFormat="1" ht="30">
+      <c r="A31" s="32" t="s">
+        <v>363</v>
+      </c>
+      <c r="B31" s="32">
+        <v>1</v>
+      </c>
+      <c r="C31" s="32">
+        <v>1</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="E31" s="33" t="s">
+        <v>300</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>301</v>
+      </c>
       <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
-      <c r="DP31" s="33"/>
-      <c r="DQ31" s="33"/>
-      <c r="DR31" s="33"/>
-      <c r="DS31" s="33"/>
-      <c r="DT31" s="33"/>
-      <c r="DU31" s="33"/>
+      <c r="H31" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="I31" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="J31" s="5">
+        <v>1</v>
+      </c>
+      <c r="K31" s="5">
+        <v>1</v>
+      </c>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="31" t="s">
+        <v>302</v>
+      </c>
+      <c r="R31" s="5"/>
+      <c r="S31" s="5"/>
+      <c r="T31" s="5"/>
+      <c r="U31" s="5"/>
+      <c r="V31" s="5"/>
+      <c r="W31" s="5"/>
+      <c r="X31" s="5"/>
+      <c r="Y31" s="5"/>
+      <c r="Z31" s="5"/>
+      <c r="AA31" s="5"/>
+      <c r="AB31" s="5"/>
+      <c r="AC31" s="5"/>
+      <c r="AD31" s="5"/>
+      <c r="AE31" s="5"/>
+      <c r="AF31" s="5"/>
+      <c r="AG31" s="5"/>
+      <c r="AH31" s="5"/>
+      <c r="AI31" s="5"/>
+      <c r="AJ31" s="5"/>
+      <c r="AK31" s="5"/>
+      <c r="AL31" s="5">
+        <v>1</v>
+      </c>
+      <c r="AM31" s="5"/>
+      <c r="AN31" s="5"/>
+      <c r="AO31" s="5"/>
+      <c r="AP31" s="5"/>
+      <c r="AQ31" s="5"/>
+      <c r="AR31" s="5"/>
+      <c r="AS31" s="5"/>
+      <c r="AT31" s="5"/>
+      <c r="AU31" s="5"/>
+      <c r="AV31" s="5"/>
+      <c r="AW31" s="5">
+        <v>1</v>
+      </c>
+      <c r="AX31" s="5"/>
+      <c r="AY31" s="5"/>
+      <c r="AZ31" s="5"/>
+      <c r="BA31" s="5"/>
+      <c r="BB31" s="5"/>
+      <c r="BC31" s="5"/>
+      <c r="BD31" s="5"/>
+      <c r="BE31" s="5"/>
+      <c r="BF31" s="5"/>
+      <c r="BG31" s="5"/>
+      <c r="BH31" s="5"/>
+      <c r="BI31" s="5"/>
+      <c r="BJ31" s="5"/>
+      <c r="BK31" s="5"/>
+      <c r="BL31" s="5"/>
+      <c r="BM31" s="5"/>
+      <c r="BN31" s="5"/>
+      <c r="BO31" s="5"/>
+      <c r="BP31" s="5"/>
+      <c r="BQ31" s="5"/>
+      <c r="BR31" s="5"/>
+      <c r="BS31" s="5"/>
+      <c r="BT31" s="5"/>
+      <c r="BU31" s="5"/>
+      <c r="BV31" s="5"/>
+      <c r="BW31" s="5"/>
+      <c r="BX31" s="5"/>
+      <c r="BY31" s="5"/>
+      <c r="BZ31" s="5"/>
+      <c r="CA31" s="5"/>
+      <c r="CB31" s="5"/>
+      <c r="CC31" s="5"/>
+      <c r="CD31" s="5"/>
+      <c r="CE31" s="5"/>
+      <c r="CF31" s="5"/>
+      <c r="CG31" s="5"/>
+      <c r="CH31" s="5"/>
+      <c r="CI31" s="5"/>
+      <c r="CJ31" s="5"/>
+      <c r="CK31" s="5"/>
+      <c r="CL31" s="5"/>
+      <c r="CM31" s="5"/>
+      <c r="CN31" s="5"/>
+      <c r="CO31" s="5"/>
+      <c r="CP31" s="5"/>
+      <c r="CQ31" s="5"/>
+      <c r="CR31" s="5"/>
+      <c r="CS31" s="5"/>
+      <c r="CT31" s="5"/>
+      <c r="CU31" s="5"/>
+      <c r="CV31" s="5"/>
+      <c r="CW31" s="5"/>
+      <c r="CX31" s="5"/>
+      <c r="CY31" s="5"/>
+      <c r="CZ31" s="5"/>
+      <c r="DA31" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="DB31" s="6">
+        <v>1</v>
+      </c>
+      <c r="DC31" s="6">
+        <v>0</v>
+      </c>
+      <c r="DD31" s="5">
+        <v>0</v>
+      </c>
+      <c r="DE31" s="5"/>
+      <c r="DF31" s="5"/>
+      <c r="DG31" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="DH31" s="5"/>
+      <c r="DI31" s="5"/>
+      <c r="DJ31" s="5"/>
+      <c r="DK31" s="5"/>
+      <c r="DL31" s="5"/>
+      <c r="DM31" s="5"/>
+      <c r="DN31" s="5"/>
+      <c r="DO31" s="5"/>
     </row>
     <row r="32" spans="1:125">
       <c r="A32" s="32"/>
@@ -3898,7 +4206,7 @@
       <c r="A37" s="32"/>
       <c r="B37" s="32"/>
       <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
+      <c r="D37" s="17"/>
       <c r="G37" s="32"/>
       <c r="H37" s="32"/>
       <c r="I37" s="32"/>
@@ -4060,7 +4368,7 @@
       <c r="DU47" s="33"/>
     </row>
     <row r="48" spans="1:125">
-      <c r="A48" s="34"/>
+      <c r="A48" s="32"/>
       <c r="B48" s="32"/>
       <c r="C48" s="32"/>
       <c r="D48" s="32"/>
@@ -4075,7 +4383,7 @@
       <c r="DU48" s="33"/>
     </row>
     <row r="49" spans="1:125">
-      <c r="A49" s="32"/>
+      <c r="A49" s="34"/>
       <c r="B49" s="32"/>
       <c r="C49" s="32"/>
       <c r="D49" s="32"/>
@@ -4118,6 +4426,21 @@
       <c r="DS51" s="33"/>
       <c r="DT51" s="33"/>
       <c r="DU51" s="33"/>
+    </row>
+    <row r="52" spans="1:125">
+      <c r="A52" s="32"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="32"/>
+      <c r="I52" s="32"/>
+      <c r="DP52" s="33"/>
+      <c r="DQ52" s="33"/>
+      <c r="DR52" s="33"/>
+      <c r="DS52" s="33"/>
+      <c r="DT52" s="33"/>
+      <c r="DU52" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4505,12 +4828,12 @@
     <row r="1" spans="1:8">
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="123" t="s">
+      <c r="E1" s="124" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
     </row>
     <row r="2" spans="1:8" ht="45">
       <c r="C2" s="74" t="s">
@@ -4809,11 +5132,11 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="C1" s="2"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="115"/>
       <c r="I1" s="101"/>
       <c r="J1" s="88"/>
     </row>
@@ -5000,15 +5323,15 @@
     <row r="1" spans="1:11" ht="26.25">
       <c r="C1" s="2"/>
       <c r="D1" s="65"/>
-      <c r="E1" s="124" t="s">
+      <c r="E1" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="124"/>
-      <c r="G1" s="124"/>
-      <c r="H1" s="124"/>
-      <c r="I1" s="124"/>
-      <c r="J1" s="124"/>
-      <c r="K1" s="124"/>
+      <c r="F1" s="125"/>
+      <c r="G1" s="125"/>
+      <c r="H1" s="125"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="125"/>
     </row>
     <row r="2" spans="1:11" ht="30">
       <c r="C2" s="75" t="s">
@@ -5393,7 +5716,7 @@
     <col min="1" max="10" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="120">
+    <row r="1" spans="1:10" ht="60">
       <c r="A1" s="100" t="s">
         <v>6</v>
       </c>
@@ -5449,8 +5772,8 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="75">
-      <c r="A3" s="125" t="s">
+    <row r="3" spans="1:10" ht="45">
+      <c r="A3" s="111" t="s">
         <v>349</v>
       </c>
       <c r="B3" s="32">
@@ -5474,7 +5797,7 @@
       </c>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="45">
+    <row r="4" spans="1:10" ht="30">
       <c r="A4" s="17" t="s">
         <v>350</v>
       </c>
@@ -5545,7 +5868,7 @@
         <v>324</v>
       </c>
       <c r="B2" s="29">
-        <f>SUM(Main!P9:P15)</f>
+        <f>SUM(Main!P10:P16)</f>
         <v>14</v>
       </c>
       <c r="E2" s="73" t="s">
@@ -5581,7 +5904,7 @@
         <v>325</v>
       </c>
       <c r="B3" s="30">
-        <f>SUM(Main!J9:J15)</f>
+        <f>SUM(Main!J10:J16)</f>
         <v>6</v>
       </c>
       <c r="E3" s="108">
@@ -5852,7 +6175,7 @@
         <v>325</v>
       </c>
       <c r="B13" s="30">
-        <f>SUM(Main!J19:J25)</f>
+        <f>SUM(Main!J20:J26)</f>
         <v>0</v>
       </c>
       <c r="E13" s="108">
@@ -6126,8 +6449,8 @@
         <v>325</v>
       </c>
       <c r="B23" s="30">
-        <f>SUM(Main!J29:J35)</f>
-        <v>0</v>
+        <f>SUM(Main!J30:J36)</f>
+        <v>2</v>
       </c>
       <c r="E23" s="38">
         <v>203</v>
@@ -6337,7 +6660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B61"/>
     </sheetView>
   </sheetViews>
@@ -10012,24 +10335,24 @@
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1">
       <c r="D1" s="73"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
-      <c r="J1" s="112"/>
-      <c r="K1" s="112"/>
-      <c r="L1" s="112"/>
-      <c r="M1" s="112"/>
-      <c r="N1" s="112"/>
-      <c r="O1" s="112"/>
-      <c r="P1" s="112"/>
-      <c r="Q1" s="112"/>
-      <c r="R1" s="112"/>
-      <c r="S1" s="112"/>
-      <c r="T1" s="112"/>
-      <c r="U1" s="112"/>
-      <c r="V1" s="112"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="113"/>
+      <c r="O1" s="113"/>
+      <c r="P1" s="113"/>
+      <c r="Q1" s="113"/>
+      <c r="R1" s="113"/>
+      <c r="S1" s="113"/>
+      <c r="T1" s="113"/>
+      <c r="U1" s="113"/>
+      <c r="V1" s="113"/>
     </row>
     <row r="2" spans="1:23" ht="96" customHeight="1">
       <c r="A2" s="42"/>
@@ -10991,37 +11314,37 @@
     <row r="1" spans="1:33" ht="15" customHeight="1">
       <c r="A1" s="42"/>
       <c r="B1" s="43"/>
-      <c r="E1" s="113" t="s">
+      <c r="E1" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
-      <c r="J1" s="112"/>
-      <c r="K1" s="112"/>
-      <c r="L1" s="112"/>
-      <c r="M1" s="112"/>
-      <c r="N1" s="112"/>
-      <c r="O1" s="112"/>
-      <c r="P1" s="112"/>
-      <c r="Q1" s="112"/>
-      <c r="R1" s="112"/>
-      <c r="S1" s="112"/>
-      <c r="T1" s="112"/>
-      <c r="U1" s="112"/>
-      <c r="V1" s="112"/>
-      <c r="W1" s="112"/>
-      <c r="X1" s="112"/>
-      <c r="Y1" s="112"/>
-      <c r="Z1" s="112"/>
-      <c r="AA1" s="112"/>
-      <c r="AB1" s="112"/>
-      <c r="AC1" s="112"/>
-      <c r="AD1" s="112"/>
-      <c r="AE1" s="112"/>
-      <c r="AF1" s="112"/>
-      <c r="AG1" s="112"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="113"/>
+      <c r="O1" s="113"/>
+      <c r="P1" s="113"/>
+      <c r="Q1" s="113"/>
+      <c r="R1" s="113"/>
+      <c r="S1" s="113"/>
+      <c r="T1" s="113"/>
+      <c r="U1" s="113"/>
+      <c r="V1" s="113"/>
+      <c r="W1" s="113"/>
+      <c r="X1" s="113"/>
+      <c r="Y1" s="113"/>
+      <c r="Z1" s="113"/>
+      <c r="AA1" s="113"/>
+      <c r="AB1" s="113"/>
+      <c r="AC1" s="113"/>
+      <c r="AD1" s="113"/>
+      <c r="AE1" s="113"/>
+      <c r="AF1" s="113"/>
+      <c r="AG1" s="113"/>
     </row>
     <row r="2" spans="1:33" ht="144" customHeight="1">
       <c r="C2" s="73" t="s">

</xml_diff>

<commit_message>
add atonic examples to dummy data
</commit_message>
<xml_diff>
--- a/tests/_dummy_data.xlsx
+++ b/tests/_dummy_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06E38C0-1D0E-416B-9844-88EF7336BDE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA15F34-E75C-4A37-A50B-8553F52575ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="368">
   <si>
     <t xml:space="preserve">Semiology </t>
   </si>
@@ -1142,6 +1142,18 @@
   </si>
   <si>
     <t>Romagnoli et al as above in adult</t>
+  </si>
+  <si>
+    <t>Marvasti's largest atonic collection</t>
+  </si>
+  <si>
+    <t>atonic collapse, loss of power</t>
+  </si>
+  <si>
+    <t>atonic</t>
+  </si>
+  <si>
+    <t>esf</t>
   </si>
 </sst>
 </file>
@@ -2346,10 +2358,10 @@
   <dimension ref="A1:DU52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="I15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A33" sqref="A33"/>
+      <selection pane="bottomRight" activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4173,13 +4185,47 @@
       <c r="DU34" s="33"/>
     </row>
     <row r="35" spans="1:125">
-      <c r="A35" s="32"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="17"/>
-      <c r="G35" s="32"/>
+      <c r="A35" s="32" t="s">
+        <v>364</v>
+      </c>
+      <c r="B35" s="32">
+        <v>999</v>
+      </c>
+      <c r="C35" s="32">
+        <v>999</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>365</v>
+      </c>
+      <c r="E35" s="33" t="s">
+        <v>366</v>
+      </c>
+      <c r="F35" s="32" t="s">
+        <v>367</v>
+      </c>
+      <c r="G35" s="32" t="s">
+        <v>116</v>
+      </c>
       <c r="H35" s="32"/>
       <c r="I35" s="32"/>
+      <c r="J35" s="5">
+        <v>2</v>
+      </c>
+      <c r="O35" s="5">
+        <v>2</v>
+      </c>
+      <c r="P35" s="5">
+        <v>999</v>
+      </c>
+      <c r="Q35" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="R35" s="5">
+        <v>900</v>
+      </c>
+      <c r="BQ35" s="5">
+        <v>99</v>
+      </c>
       <c r="DP35" s="33"/>
       <c r="DQ35" s="33"/>
       <c r="DR35" s="33"/>
@@ -6450,7 +6496,7 @@
       </c>
       <c r="B23" s="30">
         <f>SUM(Main!J30:J36)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E23" s="38">
         <v>203</v>

</xml_diff>

<commit_message>
removed duplicated precuneus from dummy data
</commit_message>
<xml_diff>
--- a/tests/_dummy_data.xlsx
+++ b/tests/_dummy_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA15F34-E75C-4A37-A50B-8553F52575ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7158D11-8087-4471-80BB-13AC28966581}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="369">
   <si>
     <t xml:space="preserve">Semiology </t>
   </si>
@@ -1154,6 +1154,9 @@
   </si>
   <si>
     <t>esf</t>
+  </si>
+  <si>
+    <t>tl</t>
   </si>
 </sst>
 </file>
@@ -2357,11 +2360,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DU52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="I15" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="M15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I35" sqref="I35"/>
+      <selection pane="bottomRight" activeCell="Q35" sqref="Q35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4237,10 +4240,29 @@
       <c r="A36" s="32"/>
       <c r="B36" s="32"/>
       <c r="C36" s="32"/>
-      <c r="D36" s="17"/>
-      <c r="G36" s="32"/>
+      <c r="D36" s="17" t="s">
+        <v>357</v>
+      </c>
+      <c r="E36" s="33" t="s">
+        <v>357</v>
+      </c>
+      <c r="F36" s="32" t="s">
+        <v>367</v>
+      </c>
+      <c r="G36" s="32" t="s">
+        <v>116</v>
+      </c>
       <c r="H36" s="32"/>
       <c r="I36" s="32"/>
+      <c r="P36" s="5">
+        <v>7</v>
+      </c>
+      <c r="Q36" s="31" t="s">
+        <v>368</v>
+      </c>
+      <c r="R36" s="5">
+        <v>7</v>
+      </c>
       <c r="DP36" s="33"/>
       <c r="DQ36" s="33"/>
       <c r="DR36" s="33"/>
@@ -4507,10 +4529,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -4806,51 +4828,29 @@
       <c r="G18" s="39"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" t="s">
-        <v>247</v>
-      </c>
-      <c r="B19" s="45">
-        <v>169</v>
-      </c>
-      <c r="C19" s="45">
-        <v>169</v>
+      <c r="A19" s="83" t="s">
+        <v>177</v>
+      </c>
+      <c r="B19" s="39">
+        <v>86</v>
+      </c>
+      <c r="C19" s="39">
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" t="s">
-        <v>248</v>
-      </c>
-      <c r="B20" s="45">
-        <v>170</v>
-      </c>
-      <c r="C20" s="45">
-        <v>170</v>
+      <c r="A20" s="83" t="s">
+        <v>184</v>
+      </c>
+      <c r="B20" s="39">
+        <v>94</v>
+      </c>
+      <c r="C20" s="39">
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="83" t="s">
-        <v>177</v>
-      </c>
-      <c r="B21" s="39">
-        <v>86</v>
-      </c>
-      <c r="C21" s="39">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="83" t="s">
-        <v>184</v>
-      </c>
-      <c r="B22" s="39">
-        <v>94</v>
-      </c>
-      <c r="C22" s="39">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="B23" s="39"/>
+      <c r="B21" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test lat not loc fix - passes still seems to have an issue  whereby some pt #s are 2 (should be 1)
</commit_message>
<xml_diff>
--- a/tests/_dummy_data.xlsx
+++ b/tests/_dummy_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5D5FA7-BBD5-43BA-851E-D5D340DC15EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A64BFD-40E6-494D-8D77-120EB894F83A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,19 +31,11 @@
     <sheet name="GIF MIXED" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="374">
   <si>
     <t xml:space="preserve">Semiology </t>
   </si>
@@ -1136,9 +1128,6 @@
     <t>precentral gyrus</t>
   </si>
   <si>
-    <t>y+CX5:DG5</t>
-  </si>
-  <si>
     <t>Romagnoli et al as above in adult</t>
   </si>
   <si>
@@ -1161,6 +1150,21 @@
   </si>
   <si>
     <t>paediatric subgroup &lt;7 years (0-6 yrs) y/n</t>
+  </si>
+  <si>
+    <t>lateralising but not localsiing</t>
+  </si>
+  <si>
+    <t>lat_not_loc</t>
+  </si>
+  <si>
+    <t>lat and loc</t>
+  </si>
+  <si>
+    <t>lat_and_loc</t>
+  </si>
+  <si>
+    <t>MTG of TL</t>
   </si>
 </sst>
 </file>
@@ -2376,10 +2380,10 @@
   <dimension ref="A1:DU52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="CW3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="J21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="CX12" sqref="CX12"/>
+      <selection pane="bottomRight" activeCell="DB26" sqref="DB26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2904,7 +2908,7 @@
         <v>107</v>
       </c>
       <c r="DA2" s="103" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="DB2" s="36" t="s">
         <v>109</v>
@@ -2925,7 +2929,7 @@
         <v>114</v>
       </c>
       <c r="DH2" s="13" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="DI2" s="12"/>
       <c r="DJ2" s="12"/>
@@ -3989,7 +3993,7 @@
         <v>0</v>
       </c>
       <c r="DG30" s="5" t="s">
-        <v>361</v>
+        <v>115</v>
       </c>
       <c r="DP30" s="33"/>
       <c r="DQ30" s="33"/>
@@ -4000,7 +4004,7 @@
     </row>
     <row r="31" spans="1:125" s="33" customFormat="1" ht="30">
       <c r="A31" s="32" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B31" s="32">
         <v>1</v>
@@ -4146,7 +4150,7 @@
       <c r="DE31" s="5"/>
       <c r="DF31" s="5"/>
       <c r="DG31" s="5" t="s">
-        <v>361</v>
+        <v>115</v>
       </c>
       <c r="DH31" s="5"/>
       <c r="DI31" s="5"/>
@@ -4204,7 +4208,7 @@
     </row>
     <row r="35" spans="1:125">
       <c r="A35" s="32" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B35" s="32">
         <v>999</v>
@@ -4213,13 +4217,13 @@
         <v>999</v>
       </c>
       <c r="D35" s="17" t="s">
+        <v>363</v>
+      </c>
+      <c r="E35" s="33" t="s">
         <v>364</v>
       </c>
-      <c r="E35" s="33" t="s">
+      <c r="F35" s="32" t="s">
         <v>365</v>
-      </c>
-      <c r="F35" s="32" t="s">
-        <v>366</v>
       </c>
       <c r="G35" s="32" t="s">
         <v>115</v>
@@ -4262,7 +4266,7 @@
         <v>356</v>
       </c>
       <c r="F36" s="32" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G36" s="32" t="s">
         <v>115</v>
@@ -4273,7 +4277,7 @@
         <v>7</v>
       </c>
       <c r="Q36" s="31" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="R36" s="5">
         <v>7</v>
@@ -4346,13 +4350,41 @@
       <c r="DU40" s="33"/>
     </row>
     <row r="41" spans="1:125">
-      <c r="A41" s="32"/>
-      <c r="B41" s="32"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="G41" s="32"/>
+      <c r="A41" s="32" t="s">
+        <v>369</v>
+      </c>
+      <c r="B41" s="32">
+        <v>1</v>
+      </c>
+      <c r="C41" s="32">
+        <v>1</v>
+      </c>
+      <c r="D41" s="32" t="s">
+        <v>370</v>
+      </c>
+      <c r="E41" s="32" t="s">
+        <v>370</v>
+      </c>
+      <c r="F41" s="32" t="s">
+        <v>365</v>
+      </c>
+      <c r="G41" s="32" t="s">
+        <v>115</v>
+      </c>
       <c r="H41" s="32"/>
       <c r="I41" s="32"/>
+      <c r="J41" s="5">
+        <v>1</v>
+      </c>
+      <c r="K41" s="5">
+        <v>1</v>
+      </c>
+      <c r="DA41" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="DF41" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="DP41" s="33"/>
       <c r="DQ41" s="33"/>
       <c r="DR41" s="33"/>
@@ -4361,13 +4393,56 @@
       <c r="DU41" s="33"/>
     </row>
     <row r="42" spans="1:125">
-      <c r="A42" s="32"/>
-      <c r="B42" s="32"/>
-      <c r="C42" s="32"/>
-      <c r="D42" s="32"/>
-      <c r="G42" s="32"/>
+      <c r="A42" s="32" t="s">
+        <v>371</v>
+      </c>
+      <c r="B42" s="32">
+        <v>1</v>
+      </c>
+      <c r="C42" s="32">
+        <v>1</v>
+      </c>
+      <c r="D42" s="32" t="s">
+        <v>372</v>
+      </c>
+      <c r="E42" s="32" t="s">
+        <v>372</v>
+      </c>
+      <c r="F42" s="32" t="s">
+        <v>365</v>
+      </c>
+      <c r="G42" s="32" t="s">
+        <v>115</v>
+      </c>
       <c r="H42" s="32"/>
       <c r="I42" s="32"/>
+      <c r="J42" s="5">
+        <v>1</v>
+      </c>
+      <c r="L42" s="5">
+        <v>1</v>
+      </c>
+      <c r="P42" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="31" t="s">
+        <v>373</v>
+      </c>
+      <c r="R42" s="5">
+        <v>1</v>
+      </c>
+      <c r="T42" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y42" s="5">
+        <v>1</v>
+      </c>
+      <c r="DA42" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="DF42" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="DP42" s="33"/>
       <c r="DQ42" s="33"/>
       <c r="DR42" s="33"/>

</xml_diff>

<commit_message>
test_latexceedsloc_3 part 1 tests the norm_ratio (odds ratio) method of Q_L when lat exceeds loc
</commit_message>
<xml_diff>
--- a/tests/_dummy_data.xlsx
+++ b/tests/_dummy_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A158E1A-1BD4-49F1-BB8A-F26C0598CBD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FB367D-0D51-4A1B-B882-09A1ADA77347}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="376">
   <si>
     <t xml:space="preserve">Semiology </t>
   </si>
@@ -1165,6 +1165,12 @@
   </si>
   <si>
     <t>MTG of TL</t>
+  </si>
+  <si>
+    <t>_loc</t>
+  </si>
+  <si>
+    <t>latexceedsloc</t>
   </si>
 </sst>
 </file>
@@ -2379,11 +2385,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DU52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="J21" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="E21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A41" sqref="A41"/>
+      <selection pane="bottomRight" activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4320,13 +4326,59 @@
       <c r="DU38" s="33"/>
     </row>
     <row r="39" spans="1:125">
-      <c r="A39" s="32"/>
-      <c r="B39" s="32"/>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
-      <c r="G39" s="32"/>
+      <c r="A39" s="32" t="s">
+        <v>375</v>
+      </c>
+      <c r="B39" s="32">
+        <v>5</v>
+      </c>
+      <c r="C39" s="32">
+        <v>500</v>
+      </c>
+      <c r="D39" s="32" t="s">
+        <v>375</v>
+      </c>
+      <c r="E39" s="32" t="s">
+        <v>375</v>
+      </c>
+      <c r="F39" s="32" t="s">
+        <v>365</v>
+      </c>
+      <c r="G39" s="32" t="s">
+        <v>115</v>
+      </c>
       <c r="H39" s="32"/>
       <c r="I39" s="32"/>
+      <c r="J39" s="5">
+        <v>500</v>
+      </c>
+      <c r="K39" s="5">
+        <v>300</v>
+      </c>
+      <c r="L39" s="5">
+        <v>200</v>
+      </c>
+      <c r="P39" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q39" s="31" t="s">
+        <v>373</v>
+      </c>
+      <c r="R39" s="5">
+        <v>2</v>
+      </c>
+      <c r="T39" s="5">
+        <v>2</v>
+      </c>
+      <c r="Y39" s="5">
+        <v>2</v>
+      </c>
+      <c r="DA39" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="DF39" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="DP39" s="33"/>
       <c r="DQ39" s="33"/>
       <c r="DR39" s="33"/>
@@ -4451,13 +4503,56 @@
       <c r="DU42" s="33"/>
     </row>
     <row r="43" spans="1:125">
-      <c r="A43" s="32"/>
-      <c r="B43" s="32"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="32"/>
-      <c r="G43" s="32"/>
+      <c r="A43" s="32" t="s">
+        <v>374</v>
+      </c>
+      <c r="B43" s="32">
+        <v>5</v>
+      </c>
+      <c r="C43" s="32">
+        <v>5</v>
+      </c>
+      <c r="D43" s="32" t="s">
+        <v>374</v>
+      </c>
+      <c r="E43" s="32" t="s">
+        <v>374</v>
+      </c>
+      <c r="F43" s="32" t="s">
+        <v>365</v>
+      </c>
+      <c r="G43" s="32" t="s">
+        <v>115</v>
+      </c>
       <c r="H43" s="32"/>
       <c r="I43" s="32"/>
+      <c r="J43" s="5">
+        <v>5</v>
+      </c>
+      <c r="K43" s="5">
+        <v>3</v>
+      </c>
+      <c r="L43" s="5">
+        <v>2</v>
+      </c>
+      <c r="P43" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q43" s="31" t="s">
+        <v>373</v>
+      </c>
+      <c r="R43" s="5">
+        <v>2</v>
+      </c>
+      <c r="T43" s="5">
+        <v>2</v>
+      </c>
+      <c r="DA43" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="DF43" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="DP43" s="33"/>
       <c r="DQ43" s="33"/>
       <c r="DR43" s="33"/>
@@ -7372,8 +7467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="F175" sqref="F175"/>
+    <sheetView topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -10366,7 +10461,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="R33" sqref="R33"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
new semiologies for pipeline testing
</commit_message>
<xml_diff>
--- a/tests/_dummy_data.xlsx
+++ b/tests/_dummy_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835B5FF4-F208-463B-8C0C-D1A3660F8DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579FDE4A-95B5-4FD0-96AC-25C8429DB538}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="379">
   <si>
     <t xml:space="preserve">Semiology </t>
   </si>
@@ -1165,6 +1165,18 @@
   </si>
   <si>
     <t>Medial Frontal (include medial premotor and its constituents as its subsets)</t>
+  </si>
+  <si>
+    <t>various</t>
+  </si>
+  <si>
+    <t>pipeline_laateralises_semioA</t>
+  </si>
+  <si>
+    <t>pipeline_notlaat_semioB</t>
+  </si>
+  <si>
+    <t>pipeline testing</t>
   </si>
 </sst>
 </file>
@@ -2377,21 +2389,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DU52"/>
+  <dimension ref="A1:DU57"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AK3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="E30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AX2" sqref="AX2"/>
+      <selection pane="bottomRight" activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="38.28515625" style="3" customWidth="1"/>
     <col min="2" max="2" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.28515625" style="33" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" style="32" customWidth="1"/>
     <col min="7" max="9" width="20.7109375" style="3" customWidth="1"/>
@@ -2472,7 +2484,7 @@
     <col min="120" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:125" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:125" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="97"/>
       <c r="C1" s="16"/>
       <c r="D1" s="114" t="s">
@@ -3013,7 +3025,6 @@
     <row r="4" spans="1:125">
       <c r="A4" s="32"/>
       <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
       <c r="D4" s="32"/>
       <c r="G4" s="32"/>
       <c r="H4" s="32"/>
@@ -3226,7 +3237,6 @@
     <row r="9" spans="1:125">
       <c r="A9" s="32"/>
       <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
       <c r="D9" s="32"/>
       <c r="G9" s="32"/>
       <c r="H9" s="32"/>
@@ -3314,7 +3324,6 @@
     <row r="11" spans="1:125">
       <c r="A11" s="17"/>
       <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
       <c r="D11" s="32" t="s">
         <v>307</v>
       </c>
@@ -3403,7 +3412,6 @@
     <row r="13" spans="1:125">
       <c r="A13" s="32"/>
       <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
       <c r="D13" s="32"/>
       <c r="G13" s="32"/>
       <c r="H13" s="32"/>
@@ -3583,7 +3591,6 @@
     <row r="17" spans="1:125">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
       <c r="D17" s="32"/>
       <c r="G17" s="32"/>
       <c r="H17" s="32"/>
@@ -3598,7 +3605,6 @@
     <row r="18" spans="1:125">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
       <c r="D18" s="32"/>
       <c r="G18" s="32"/>
       <c r="H18" s="32"/>
@@ -3613,7 +3619,6 @@
     <row r="19" spans="1:125">
       <c r="A19" s="32"/>
       <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
       <c r="D19" s="32"/>
       <c r="G19" s="32"/>
       <c r="H19" s="32"/>
@@ -3628,7 +3633,6 @@
     <row r="20" spans="1:125">
       <c r="A20" s="32"/>
       <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
       <c r="D20" s="32"/>
       <c r="G20" s="32"/>
       <c r="H20" s="32"/>
@@ -3643,7 +3647,6 @@
     <row r="21" spans="1:125">
       <c r="A21" s="32"/>
       <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
       <c r="D21" s="32"/>
       <c r="G21" s="32"/>
       <c r="H21" s="32"/>
@@ -3658,7 +3661,6 @@
     <row r="22" spans="1:125">
       <c r="A22" s="32"/>
       <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
       <c r="D22" s="32"/>
       <c r="G22" s="32"/>
       <c r="H22" s="32"/>
@@ -3823,7 +3825,6 @@
     <row r="26" spans="1:125">
       <c r="A26" s="32"/>
       <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
       <c r="D26" s="17"/>
       <c r="G26" s="32"/>
       <c r="H26" s="32"/>
@@ -3838,7 +3839,6 @@
     <row r="27" spans="1:125">
       <c r="A27" s="32"/>
       <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
       <c r="D27" s="17"/>
       <c r="G27" s="32"/>
       <c r="H27" s="32"/>
@@ -4164,7 +4164,6 @@
     <row r="32" spans="1:125">
       <c r="A32" s="32"/>
       <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
       <c r="D32" s="17"/>
       <c r="G32" s="32"/>
       <c r="H32" s="32"/>
@@ -4179,7 +4178,6 @@
     <row r="33" spans="1:125">
       <c r="A33" s="32"/>
       <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
       <c r="D33" s="17"/>
       <c r="G33" s="32"/>
       <c r="H33" s="32"/>
@@ -4194,7 +4192,6 @@
     <row r="34" spans="1:125">
       <c r="A34" s="32"/>
       <c r="B34" s="32"/>
-      <c r="C34" s="32"/>
       <c r="D34" s="17"/>
       <c r="G34" s="32"/>
       <c r="H34" s="32"/>
@@ -4258,7 +4255,6 @@
     <row r="36" spans="1:125">
       <c r="A36" s="32"/>
       <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
       <c r="D36" s="17" t="s">
         <v>352</v>
       </c>
@@ -4292,7 +4288,6 @@
     <row r="37" spans="1:125">
       <c r="A37" s="32"/>
       <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
       <c r="D37" s="17"/>
       <c r="G37" s="32"/>
       <c r="H37" s="32"/>
@@ -4307,7 +4302,6 @@
     <row r="38" spans="1:125">
       <c r="A38" s="32"/>
       <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
       <c r="D38" s="32"/>
       <c r="G38" s="32"/>
       <c r="H38" s="32"/>
@@ -4383,7 +4377,6 @@
     <row r="40" spans="1:125">
       <c r="A40" s="32"/>
       <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
       <c r="D40" s="32"/>
       <c r="G40" s="32"/>
       <c r="H40" s="32"/>
@@ -4557,7 +4550,6 @@
     <row r="44" spans="1:125">
       <c r="A44" s="32"/>
       <c r="B44" s="32"/>
-      <c r="C44" s="32"/>
       <c r="D44" s="32"/>
       <c r="G44" s="32"/>
       <c r="H44" s="32"/>
@@ -4572,7 +4564,6 @@
     <row r="45" spans="1:125">
       <c r="A45" s="32"/>
       <c r="B45" s="32"/>
-      <c r="C45" s="32"/>
       <c r="D45" s="32"/>
       <c r="G45" s="32"/>
       <c r="H45" s="32"/>
@@ -4587,7 +4578,6 @@
     <row r="46" spans="1:125">
       <c r="A46" s="32"/>
       <c r="B46" s="32"/>
-      <c r="C46" s="32"/>
       <c r="D46" s="32"/>
       <c r="G46" s="32"/>
       <c r="H46" s="32"/>
@@ -4602,7 +4592,6 @@
     <row r="47" spans="1:125">
       <c r="A47" s="32"/>
       <c r="B47" s="32"/>
-      <c r="C47" s="32"/>
       <c r="D47" s="32"/>
       <c r="G47" s="32"/>
       <c r="H47" s="32"/>
@@ -4616,9 +4605,10 @@
     </row>
     <row r="48" spans="1:125">
       <c r="A48" s="32"/>
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
+      <c r="B48"/>
+      <c r="C48" s="39"/>
+      <c r="D48"/>
+      <c r="E48"/>
       <c r="G48" s="32"/>
       <c r="H48" s="32"/>
       <c r="I48" s="32"/>
@@ -4630,13 +4620,88 @@
       <c r="DU48" s="33"/>
     </row>
     <row r="49" spans="1:125">
-      <c r="A49" s="34"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="G49" s="32"/>
+      <c r="A49" s="34" t="s">
+        <v>378</v>
+      </c>
+      <c r="B49"/>
+      <c r="C49" s="39">
+        <v>10</v>
+      </c>
+      <c r="D49" t="s">
+        <v>376</v>
+      </c>
+      <c r="E49"/>
+      <c r="F49" s="32" t="s">
+        <v>361</v>
+      </c>
+      <c r="G49" s="32" t="s">
+        <v>112</v>
+      </c>
       <c r="H49" s="32"/>
       <c r="I49" s="32"/>
+      <c r="J49" s="5">
+        <v>9</v>
+      </c>
+      <c r="K49" s="5">
+        <v>8</v>
+      </c>
+      <c r="L49" s="5">
+        <v>1</v>
+      </c>
+      <c r="P49" s="5">
+        <v>10</v>
+      </c>
+      <c r="Q49" s="31" t="s">
+        <v>375</v>
+      </c>
+      <c r="R49" s="5">
+        <v>3</v>
+      </c>
+      <c r="T49" s="5">
+        <v>3</v>
+      </c>
+      <c r="U49" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y49" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL49" s="5">
+        <v>4</v>
+      </c>
+      <c r="AQ49" s="5">
+        <v>2</v>
+      </c>
+      <c r="AR49" s="5">
+        <v>2</v>
+      </c>
+      <c r="AV49" s="5">
+        <v>2</v>
+      </c>
+      <c r="BQ49" s="5">
+        <v>1</v>
+      </c>
+      <c r="BW49" s="5">
+        <v>1</v>
+      </c>
+      <c r="BY49" s="5">
+        <v>1</v>
+      </c>
+      <c r="CB49" s="5">
+        <v>1</v>
+      </c>
+      <c r="CN49" s="5">
+        <v>1</v>
+      </c>
+      <c r="CO49" s="5">
+        <v>1</v>
+      </c>
+      <c r="DA49" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="DF49" s="5" t="s">
+        <v>112</v>
+      </c>
       <c r="DP49" s="33"/>
       <c r="DQ49" s="33"/>
       <c r="DR49" s="33"/>
@@ -4646,9 +4711,10 @@
     </row>
     <row r="50" spans="1:125">
       <c r="A50" s="32"/>
-      <c r="B50" s="32"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
+      <c r="B50"/>
+      <c r="C50" s="39"/>
+      <c r="D50"/>
+      <c r="E50"/>
       <c r="G50" s="32"/>
       <c r="H50" s="32"/>
       <c r="I50" s="32"/>
@@ -4661,12 +4727,76 @@
     </row>
     <row r="51" spans="1:125">
       <c r="A51" s="32"/>
-      <c r="B51" s="32"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="32"/>
-      <c r="G51" s="32"/>
+      <c r="B51"/>
+      <c r="C51" s="39">
+        <v>10</v>
+      </c>
+      <c r="D51" t="s">
+        <v>377</v>
+      </c>
+      <c r="E51"/>
+      <c r="F51" s="32" t="s">
+        <v>361</v>
+      </c>
+      <c r="G51" s="32" t="s">
+        <v>112</v>
+      </c>
       <c r="H51" s="32"/>
       <c r="I51" s="32"/>
+      <c r="P51" s="5">
+        <v>10</v>
+      </c>
+      <c r="Q51" s="31" t="s">
+        <v>375</v>
+      </c>
+      <c r="R51" s="5">
+        <v>3</v>
+      </c>
+      <c r="T51" s="5">
+        <v>3</v>
+      </c>
+      <c r="U51" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y51" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL51" s="5">
+        <v>4</v>
+      </c>
+      <c r="AQ51" s="5">
+        <v>2</v>
+      </c>
+      <c r="AR51" s="5">
+        <v>2</v>
+      </c>
+      <c r="AV51" s="5">
+        <v>2</v>
+      </c>
+      <c r="BQ51" s="5">
+        <v>1</v>
+      </c>
+      <c r="BW51" s="5">
+        <v>1</v>
+      </c>
+      <c r="BY51" s="5">
+        <v>1</v>
+      </c>
+      <c r="CB51" s="5">
+        <v>1</v>
+      </c>
+      <c r="CN51" s="5">
+        <v>1</v>
+      </c>
+      <c r="CO51" s="5">
+        <v>1</v>
+      </c>
+      <c r="DA51" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="DF51" s="5" t="s">
+        <v>112</v>
+      </c>
       <c r="DP51" s="33"/>
       <c r="DQ51" s="33"/>
       <c r="DR51" s="33"/>
@@ -4676,9 +4806,10 @@
     </row>
     <row r="52" spans="1:125">
       <c r="A52" s="32"/>
-      <c r="B52" s="32"/>
-      <c r="C52" s="32"/>
-      <c r="D52" s="32"/>
+      <c r="B52"/>
+      <c r="C52" s="39"/>
+      <c r="D52"/>
+      <c r="E52"/>
       <c r="G52" s="32"/>
       <c r="H52" s="32"/>
       <c r="I52" s="32"/>
@@ -4688,6 +4819,36 @@
       <c r="DS52" s="33"/>
       <c r="DT52" s="33"/>
       <c r="DU52" s="33"/>
+    </row>
+    <row r="53" spans="1:125">
+      <c r="B53"/>
+      <c r="C53" s="39"/>
+      <c r="D53"/>
+      <c r="E53"/>
+    </row>
+    <row r="54" spans="1:125">
+      <c r="B54"/>
+      <c r="C54" s="39"/>
+      <c r="D54"/>
+      <c r="E54"/>
+    </row>
+    <row r="55" spans="1:125">
+      <c r="B55"/>
+      <c r="C55" s="39"/>
+      <c r="D55"/>
+      <c r="E55"/>
+    </row>
+    <row r="56" spans="1:125">
+      <c r="B56"/>
+      <c r="C56" s="39"/>
+      <c r="D56"/>
+      <c r="E56"/>
+    </row>
+    <row r="57" spans="1:125">
+      <c r="B57"/>
+      <c r="C57" s="39"/>
+      <c r="D57"/>
+      <c r="E57"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -11453,7 +11614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AG324"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add semioC for test_prelim5_ql_50_50 related to #94
</commit_message>
<xml_diff>
--- a/tests/_dummy_data.xlsx
+++ b/tests/_dummy_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579FDE4A-95B5-4FD0-96AC-25C8429DB538}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98D50DA-1BEF-414A-A41F-79C14509BEAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="381">
   <si>
     <t xml:space="preserve">Semiology </t>
   </si>
@@ -1177,6 +1177,12 @@
   </si>
   <si>
     <t>pipeline testing</t>
+  </si>
+  <si>
+    <t>pipeline_50_50_laateralises_semioC</t>
+  </si>
+  <si>
+    <t>as above various</t>
   </si>
 </sst>
 </file>
@@ -2392,10 +2398,10 @@
   <dimension ref="A1:DU57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="P30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D57" sqref="D57"/>
+      <selection pane="bottomRight" activeCell="R55" sqref="R55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2403,7 +2409,7 @@
     <col min="1" max="1" width="38.28515625" style="3" customWidth="1"/>
     <col min="2" max="2" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" style="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.28515625" style="33" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" style="32" customWidth="1"/>
     <col min="7" max="9" width="20.7109375" style="3" customWidth="1"/>
@@ -4747,7 +4753,7 @@
         <v>10</v>
       </c>
       <c r="Q51" s="31" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="R51" s="5">
         <v>3</v>
@@ -4822,19 +4828,86 @@
     </row>
     <row r="53" spans="1:125">
       <c r="B53"/>
-      <c r="C53" s="39"/>
-      <c r="D53"/>
+      <c r="C53" s="39">
+        <v>30</v>
+      </c>
+      <c r="D53" t="s">
+        <v>379</v>
+      </c>
       <c r="E53"/>
+      <c r="J53" s="5">
+        <v>20</v>
+      </c>
+      <c r="K53" s="5">
+        <v>10</v>
+      </c>
+      <c r="L53" s="5">
+        <v>10</v>
+      </c>
+      <c r="P53" s="5">
+        <v>30</v>
+      </c>
+      <c r="Q53" s="31" t="s">
+        <v>380</v>
+      </c>
+      <c r="R53" s="5">
+        <v>3</v>
+      </c>
+      <c r="T53" s="5">
+        <v>3</v>
+      </c>
+      <c r="U53" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y53" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL53" s="5">
+        <v>4</v>
+      </c>
+      <c r="AQ53" s="5">
+        <v>2</v>
+      </c>
+      <c r="AR53" s="5">
+        <v>2</v>
+      </c>
+      <c r="AV53" s="5">
+        <v>2</v>
+      </c>
+      <c r="BQ53" s="5">
+        <v>1</v>
+      </c>
+      <c r="BW53" s="5">
+        <v>1</v>
+      </c>
+      <c r="BY53" s="5">
+        <v>1</v>
+      </c>
+      <c r="CB53" s="5">
+        <v>1</v>
+      </c>
+      <c r="CN53" s="5">
+        <v>1</v>
+      </c>
+      <c r="CO53" s="5">
+        <v>1</v>
+      </c>
+      <c r="DA53" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="DF53" s="5" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="54" spans="1:125">
       <c r="B54"/>
-      <c r="C54" s="39"/>
+      <c r="C54"/>
       <c r="D54"/>
       <c r="E54"/>
     </row>
     <row r="55" spans="1:125">
       <c r="B55"/>
-      <c r="C55" s="39"/>
+      <c r="C55"/>
       <c r="D55"/>
       <c r="E55"/>
     </row>
@@ -7622,8 +7695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D169"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D61" sqref="D60:D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Pipeline testing (#189) fixes #94
* preliminary tests for pipeline sequence testing

* new semiologies for pipeline testing

* test pipeline shapes: query_lateralisation
with and without lateralising data

* test pipeline GIFs sameL query_lateralisation()
with and without lateralising data

* test pipeline GIFvalues diff: query_lateralisation
with and without lat

* compare pipelines 1 corrected
related to #94

* add semioC for test_prelim5_ql_50_50
related to #94

* more detailed pipeline testing
related #94

* pipeline sequence testing complete
</commit_message>
<xml_diff>
--- a/tests/_dummy_data.xlsx
+++ b/tests/_dummy_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835B5FF4-F208-463B-8C0C-D1A3660F8DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98D50DA-1BEF-414A-A41F-79C14509BEAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="381">
   <si>
     <t xml:space="preserve">Semiology </t>
   </si>
@@ -1165,6 +1165,24 @@
   </si>
   <si>
     <t>Medial Frontal (include medial premotor and its constituents as its subsets)</t>
+  </si>
+  <si>
+    <t>various</t>
+  </si>
+  <si>
+    <t>pipeline_laateralises_semioA</t>
+  </si>
+  <si>
+    <t>pipeline_notlaat_semioB</t>
+  </si>
+  <si>
+    <t>pipeline testing</t>
+  </si>
+  <si>
+    <t>pipeline_50_50_laateralises_semioC</t>
+  </si>
+  <si>
+    <t>as above various</t>
   </si>
 </sst>
 </file>
@@ -2377,21 +2395,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DU52"/>
+  <dimension ref="A1:DU57"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AK3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="P30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AX2" sqref="AX2"/>
+      <selection pane="bottomRight" activeCell="R55" sqref="R55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="38.28515625" style="3" customWidth="1"/>
     <col min="2" max="2" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.28515625" style="33" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" style="32" customWidth="1"/>
     <col min="7" max="9" width="20.7109375" style="3" customWidth="1"/>
@@ -2472,7 +2490,7 @@
     <col min="120" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:125" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:125" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="97"/>
       <c r="C1" s="16"/>
       <c r="D1" s="114" t="s">
@@ -3013,7 +3031,6 @@
     <row r="4" spans="1:125">
       <c r="A4" s="32"/>
       <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
       <c r="D4" s="32"/>
       <c r="G4" s="32"/>
       <c r="H4" s="32"/>
@@ -3226,7 +3243,6 @@
     <row r="9" spans="1:125">
       <c r="A9" s="32"/>
       <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
       <c r="D9" s="32"/>
       <c r="G9" s="32"/>
       <c r="H9" s="32"/>
@@ -3314,7 +3330,6 @@
     <row r="11" spans="1:125">
       <c r="A11" s="17"/>
       <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
       <c r="D11" s="32" t="s">
         <v>307</v>
       </c>
@@ -3403,7 +3418,6 @@
     <row r="13" spans="1:125">
       <c r="A13" s="32"/>
       <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
       <c r="D13" s="32"/>
       <c r="G13" s="32"/>
       <c r="H13" s="32"/>
@@ -3583,7 +3597,6 @@
     <row r="17" spans="1:125">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
       <c r="D17" s="32"/>
       <c r="G17" s="32"/>
       <c r="H17" s="32"/>
@@ -3598,7 +3611,6 @@
     <row r="18" spans="1:125">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
       <c r="D18" s="32"/>
       <c r="G18" s="32"/>
       <c r="H18" s="32"/>
@@ -3613,7 +3625,6 @@
     <row r="19" spans="1:125">
       <c r="A19" s="32"/>
       <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
       <c r="D19" s="32"/>
       <c r="G19" s="32"/>
       <c r="H19" s="32"/>
@@ -3628,7 +3639,6 @@
     <row r="20" spans="1:125">
       <c r="A20" s="32"/>
       <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
       <c r="D20" s="32"/>
       <c r="G20" s="32"/>
       <c r="H20" s="32"/>
@@ -3643,7 +3653,6 @@
     <row r="21" spans="1:125">
       <c r="A21" s="32"/>
       <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
       <c r="D21" s="32"/>
       <c r="G21" s="32"/>
       <c r="H21" s="32"/>
@@ -3658,7 +3667,6 @@
     <row r="22" spans="1:125">
       <c r="A22" s="32"/>
       <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
       <c r="D22" s="32"/>
       <c r="G22" s="32"/>
       <c r="H22" s="32"/>
@@ -3823,7 +3831,6 @@
     <row r="26" spans="1:125">
       <c r="A26" s="32"/>
       <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
       <c r="D26" s="17"/>
       <c r="G26" s="32"/>
       <c r="H26" s="32"/>
@@ -3838,7 +3845,6 @@
     <row r="27" spans="1:125">
       <c r="A27" s="32"/>
       <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
       <c r="D27" s="17"/>
       <c r="G27" s="32"/>
       <c r="H27" s="32"/>
@@ -4164,7 +4170,6 @@
     <row r="32" spans="1:125">
       <c r="A32" s="32"/>
       <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
       <c r="D32" s="17"/>
       <c r="G32" s="32"/>
       <c r="H32" s="32"/>
@@ -4179,7 +4184,6 @@
     <row r="33" spans="1:125">
       <c r="A33" s="32"/>
       <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
       <c r="D33" s="17"/>
       <c r="G33" s="32"/>
       <c r="H33" s="32"/>
@@ -4194,7 +4198,6 @@
     <row r="34" spans="1:125">
       <c r="A34" s="32"/>
       <c r="B34" s="32"/>
-      <c r="C34" s="32"/>
       <c r="D34" s="17"/>
       <c r="G34" s="32"/>
       <c r="H34" s="32"/>
@@ -4258,7 +4261,6 @@
     <row r="36" spans="1:125">
       <c r="A36" s="32"/>
       <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
       <c r="D36" s="17" t="s">
         <v>352</v>
       </c>
@@ -4292,7 +4294,6 @@
     <row r="37" spans="1:125">
       <c r="A37" s="32"/>
       <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
       <c r="D37" s="17"/>
       <c r="G37" s="32"/>
       <c r="H37" s="32"/>
@@ -4307,7 +4308,6 @@
     <row r="38" spans="1:125">
       <c r="A38" s="32"/>
       <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
       <c r="D38" s="32"/>
       <c r="G38" s="32"/>
       <c r="H38" s="32"/>
@@ -4383,7 +4383,6 @@
     <row r="40" spans="1:125">
       <c r="A40" s="32"/>
       <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
       <c r="D40" s="32"/>
       <c r="G40" s="32"/>
       <c r="H40" s="32"/>
@@ -4557,7 +4556,6 @@
     <row r="44" spans="1:125">
       <c r="A44" s="32"/>
       <c r="B44" s="32"/>
-      <c r="C44" s="32"/>
       <c r="D44" s="32"/>
       <c r="G44" s="32"/>
       <c r="H44" s="32"/>
@@ -4572,7 +4570,6 @@
     <row r="45" spans="1:125">
       <c r="A45" s="32"/>
       <c r="B45" s="32"/>
-      <c r="C45" s="32"/>
       <c r="D45" s="32"/>
       <c r="G45" s="32"/>
       <c r="H45" s="32"/>
@@ -4587,7 +4584,6 @@
     <row r="46" spans="1:125">
       <c r="A46" s="32"/>
       <c r="B46" s="32"/>
-      <c r="C46" s="32"/>
       <c r="D46" s="32"/>
       <c r="G46" s="32"/>
       <c r="H46" s="32"/>
@@ -4602,7 +4598,6 @@
     <row r="47" spans="1:125">
       <c r="A47" s="32"/>
       <c r="B47" s="32"/>
-      <c r="C47" s="32"/>
       <c r="D47" s="32"/>
       <c r="G47" s="32"/>
       <c r="H47" s="32"/>
@@ -4616,9 +4611,10 @@
     </row>
     <row r="48" spans="1:125">
       <c r="A48" s="32"/>
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
+      <c r="B48"/>
+      <c r="C48" s="39"/>
+      <c r="D48"/>
+      <c r="E48"/>
       <c r="G48" s="32"/>
       <c r="H48" s="32"/>
       <c r="I48" s="32"/>
@@ -4630,13 +4626,88 @@
       <c r="DU48" s="33"/>
     </row>
     <row r="49" spans="1:125">
-      <c r="A49" s="34"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="G49" s="32"/>
+      <c r="A49" s="34" t="s">
+        <v>378</v>
+      </c>
+      <c r="B49"/>
+      <c r="C49" s="39">
+        <v>10</v>
+      </c>
+      <c r="D49" t="s">
+        <v>376</v>
+      </c>
+      <c r="E49"/>
+      <c r="F49" s="32" t="s">
+        <v>361</v>
+      </c>
+      <c r="G49" s="32" t="s">
+        <v>112</v>
+      </c>
       <c r="H49" s="32"/>
       <c r="I49" s="32"/>
+      <c r="J49" s="5">
+        <v>9</v>
+      </c>
+      <c r="K49" s="5">
+        <v>8</v>
+      </c>
+      <c r="L49" s="5">
+        <v>1</v>
+      </c>
+      <c r="P49" s="5">
+        <v>10</v>
+      </c>
+      <c r="Q49" s="31" t="s">
+        <v>375</v>
+      </c>
+      <c r="R49" s="5">
+        <v>3</v>
+      </c>
+      <c r="T49" s="5">
+        <v>3</v>
+      </c>
+      <c r="U49" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y49" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL49" s="5">
+        <v>4</v>
+      </c>
+      <c r="AQ49" s="5">
+        <v>2</v>
+      </c>
+      <c r="AR49" s="5">
+        <v>2</v>
+      </c>
+      <c r="AV49" s="5">
+        <v>2</v>
+      </c>
+      <c r="BQ49" s="5">
+        <v>1</v>
+      </c>
+      <c r="BW49" s="5">
+        <v>1</v>
+      </c>
+      <c r="BY49" s="5">
+        <v>1</v>
+      </c>
+      <c r="CB49" s="5">
+        <v>1</v>
+      </c>
+      <c r="CN49" s="5">
+        <v>1</v>
+      </c>
+      <c r="CO49" s="5">
+        <v>1</v>
+      </c>
+      <c r="DA49" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="DF49" s="5" t="s">
+        <v>112</v>
+      </c>
       <c r="DP49" s="33"/>
       <c r="DQ49" s="33"/>
       <c r="DR49" s="33"/>
@@ -4646,9 +4717,10 @@
     </row>
     <row r="50" spans="1:125">
       <c r="A50" s="32"/>
-      <c r="B50" s="32"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
+      <c r="B50"/>
+      <c r="C50" s="39"/>
+      <c r="D50"/>
+      <c r="E50"/>
       <c r="G50" s="32"/>
       <c r="H50" s="32"/>
       <c r="I50" s="32"/>
@@ -4661,12 +4733,76 @@
     </row>
     <row r="51" spans="1:125">
       <c r="A51" s="32"/>
-      <c r="B51" s="32"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="32"/>
-      <c r="G51" s="32"/>
+      <c r="B51"/>
+      <c r="C51" s="39">
+        <v>10</v>
+      </c>
+      <c r="D51" t="s">
+        <v>377</v>
+      </c>
+      <c r="E51"/>
+      <c r="F51" s="32" t="s">
+        <v>361</v>
+      </c>
+      <c r="G51" s="32" t="s">
+        <v>112</v>
+      </c>
       <c r="H51" s="32"/>
       <c r="I51" s="32"/>
+      <c r="P51" s="5">
+        <v>10</v>
+      </c>
+      <c r="Q51" s="31" t="s">
+        <v>380</v>
+      </c>
+      <c r="R51" s="5">
+        <v>3</v>
+      </c>
+      <c r="T51" s="5">
+        <v>3</v>
+      </c>
+      <c r="U51" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y51" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL51" s="5">
+        <v>4</v>
+      </c>
+      <c r="AQ51" s="5">
+        <v>2</v>
+      </c>
+      <c r="AR51" s="5">
+        <v>2</v>
+      </c>
+      <c r="AV51" s="5">
+        <v>2</v>
+      </c>
+      <c r="BQ51" s="5">
+        <v>1</v>
+      </c>
+      <c r="BW51" s="5">
+        <v>1</v>
+      </c>
+      <c r="BY51" s="5">
+        <v>1</v>
+      </c>
+      <c r="CB51" s="5">
+        <v>1</v>
+      </c>
+      <c r="CN51" s="5">
+        <v>1</v>
+      </c>
+      <c r="CO51" s="5">
+        <v>1</v>
+      </c>
+      <c r="DA51" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="DF51" s="5" t="s">
+        <v>112</v>
+      </c>
       <c r="DP51" s="33"/>
       <c r="DQ51" s="33"/>
       <c r="DR51" s="33"/>
@@ -4676,9 +4812,10 @@
     </row>
     <row r="52" spans="1:125">
       <c r="A52" s="32"/>
-      <c r="B52" s="32"/>
-      <c r="C52" s="32"/>
-      <c r="D52" s="32"/>
+      <c r="B52"/>
+      <c r="C52" s="39"/>
+      <c r="D52"/>
+      <c r="E52"/>
       <c r="G52" s="32"/>
       <c r="H52" s="32"/>
       <c r="I52" s="32"/>
@@ -4688,6 +4825,103 @@
       <c r="DS52" s="33"/>
       <c r="DT52" s="33"/>
       <c r="DU52" s="33"/>
+    </row>
+    <row r="53" spans="1:125">
+      <c r="B53"/>
+      <c r="C53" s="39">
+        <v>30</v>
+      </c>
+      <c r="D53" t="s">
+        <v>379</v>
+      </c>
+      <c r="E53"/>
+      <c r="J53" s="5">
+        <v>20</v>
+      </c>
+      <c r="K53" s="5">
+        <v>10</v>
+      </c>
+      <c r="L53" s="5">
+        <v>10</v>
+      </c>
+      <c r="P53" s="5">
+        <v>30</v>
+      </c>
+      <c r="Q53" s="31" t="s">
+        <v>380</v>
+      </c>
+      <c r="R53" s="5">
+        <v>3</v>
+      </c>
+      <c r="T53" s="5">
+        <v>3</v>
+      </c>
+      <c r="U53" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y53" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL53" s="5">
+        <v>4</v>
+      </c>
+      <c r="AQ53" s="5">
+        <v>2</v>
+      </c>
+      <c r="AR53" s="5">
+        <v>2</v>
+      </c>
+      <c r="AV53" s="5">
+        <v>2</v>
+      </c>
+      <c r="BQ53" s="5">
+        <v>1</v>
+      </c>
+      <c r="BW53" s="5">
+        <v>1</v>
+      </c>
+      <c r="BY53" s="5">
+        <v>1</v>
+      </c>
+      <c r="CB53" s="5">
+        <v>1</v>
+      </c>
+      <c r="CN53" s="5">
+        <v>1</v>
+      </c>
+      <c r="CO53" s="5">
+        <v>1</v>
+      </c>
+      <c r="DA53" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="DF53" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" spans="1:125">
+      <c r="B54"/>
+      <c r="C54"/>
+      <c r="D54"/>
+      <c r="E54"/>
+    </row>
+    <row r="55" spans="1:125">
+      <c r="B55"/>
+      <c r="C55"/>
+      <c r="D55"/>
+      <c r="E55"/>
+    </row>
+    <row r="56" spans="1:125">
+      <c r="B56"/>
+      <c r="C56" s="39"/>
+      <c r="D56"/>
+      <c r="E56"/>
+    </row>
+    <row r="57" spans="1:125">
+      <c r="B57"/>
+      <c r="C57" s="39"/>
+      <c r="D57"/>
+      <c r="E57"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -7461,8 +7695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D169"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D61" sqref="D60:D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -11453,7 +11687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AG324"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update test pipeline and the loc and lat values
</commit_message>
<xml_diff>
--- a/tests/_dummy_data.xlsx
+++ b/tests/_dummy_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98D50DA-1BEF-414A-A41F-79C14509BEAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41C953F-FDC9-4AAE-96AC-49D0EC77BB1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="381">
   <si>
     <t xml:space="preserve">Semiology </t>
   </si>
@@ -2398,10 +2398,10 @@
   <dimension ref="A1:DU57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="P30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="H30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R55" sqref="R55"/>
+      <selection pane="bottomRight" activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4835,17 +4835,23 @@
         <v>379</v>
       </c>
       <c r="E53"/>
+      <c r="F53" s="32" t="s">
+        <v>361</v>
+      </c>
+      <c r="G53" s="32" t="s">
+        <v>112</v>
+      </c>
       <c r="J53" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K53" s="5">
+        <v>5</v>
+      </c>
+      <c r="L53" s="5">
+        <v>5</v>
+      </c>
+      <c r="P53" s="5">
         <v>10</v>
-      </c>
-      <c r="L53" s="5">
-        <v>10</v>
-      </c>
-      <c r="P53" s="5">
-        <v>30</v>
       </c>
       <c r="Q53" s="31" t="s">
         <v>380</v>

</xml_diff>

<commit_message>
minor dummy data update
</commit_message>
<xml_diff>
--- a/tests/_dummy_data.xlsx
+++ b/tests/_dummy_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41C953F-FDC9-4AAE-96AC-49D0EC77BB1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9567653-48DD-4BC6-990A-E5AB9E4971B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2401,7 +2401,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="H30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I50" sqref="I50"/>
+      <selection pane="bottomRight" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4829,7 +4829,7 @@
     <row r="53" spans="1:125">
       <c r="B53"/>
       <c r="C53" s="39">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D53" t="s">
         <v>379</v>

</xml_diff>

<commit_message>
added IVL_1 and ILV_4 semiologies to dummy data related to #169
</commit_message>
<xml_diff>
--- a/tests/_dummy_data.xlsx
+++ b/tests/_dummy_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0ABA2F-17A5-4144-ADB5-FE55489721C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31544ACE-914C-487D-A8B0-3F9AE4FDBEFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="384">
   <si>
     <t xml:space="preserve">Semiology </t>
   </si>
@@ -1183,6 +1183,15 @@
   </si>
   <si>
     <t>as above various</t>
+  </si>
+  <si>
+    <t>ILV_4</t>
+  </si>
+  <si>
+    <t>ILV_1</t>
+  </si>
+  <si>
+    <t>4 separate lobes</t>
   </si>
 </sst>
 </file>
@@ -2398,10 +2407,10 @@
   <dimension ref="A1:DU57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="H30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="F36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D56" sqref="D56"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4907,21 +4916,123 @@
     </row>
     <row r="54" spans="1:125">
       <c r="B54"/>
-      <c r="C54"/>
+      <c r="C54" s="39"/>
       <c r="D54"/>
       <c r="E54"/>
     </row>
     <row r="55" spans="1:125">
       <c r="B55"/>
-      <c r="C55"/>
-      <c r="D55"/>
-      <c r="E55"/>
+      <c r="C55" s="39">
+        <v>4</v>
+      </c>
+      <c r="D55" t="s">
+        <v>381</v>
+      </c>
+      <c r="E55" t="s">
+        <v>381</v>
+      </c>
+      <c r="F55" s="32" t="s">
+        <v>361</v>
+      </c>
+      <c r="G55" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="P55" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q55" s="31" t="s">
+        <v>383</v>
+      </c>
+      <c r="R55" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA55" s="5">
+        <v>1</v>
+      </c>
+      <c r="AH55" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL55" s="5">
+        <v>1</v>
+      </c>
+      <c r="AW55" s="5">
+        <v>1</v>
+      </c>
+      <c r="BQ55" s="5">
+        <v>1</v>
+      </c>
+      <c r="BY55" s="5">
+        <v>1</v>
+      </c>
+      <c r="CD55" s="5">
+        <v>1</v>
+      </c>
+      <c r="CF55" s="5">
+        <v>1</v>
+      </c>
+      <c r="DA55" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="DF55" s="5" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="56" spans="1:125">
       <c r="B56"/>
-      <c r="C56" s="39"/>
-      <c r="D56"/>
-      <c r="E56"/>
+      <c r="C56" s="39">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
+        <v>382</v>
+      </c>
+      <c r="E56" t="s">
+        <v>382</v>
+      </c>
+      <c r="F56" s="32" t="s">
+        <v>361</v>
+      </c>
+      <c r="G56" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="P56" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q56" s="31" t="s">
+        <v>383</v>
+      </c>
+      <c r="R56" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA56" s="5">
+        <v>1</v>
+      </c>
+      <c r="AH56" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL56" s="5">
+        <v>1</v>
+      </c>
+      <c r="AW56" s="5">
+        <v>1</v>
+      </c>
+      <c r="BQ56" s="5">
+        <v>1</v>
+      </c>
+      <c r="BY56" s="5">
+        <v>1</v>
+      </c>
+      <c r="CD56" s="5">
+        <v>1</v>
+      </c>
+      <c r="CF56" s="5">
+        <v>1</v>
+      </c>
+      <c r="DA56" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="DF56" s="5" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="57" spans="1:125">
       <c r="B57"/>

</xml_diff>

<commit_message>
fix dummy_data postcode localisations FL data related to #94
</commit_message>
<xml_diff>
--- a/tests/_dummy_data.xlsx
+++ b/tests/_dummy_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31544ACE-914C-487D-A8B0-3F9AE4FDBEFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497636CA-478E-4B47-80AF-7EECE4606478}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2407,10 +2407,10 @@
   <dimension ref="A1:DU57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="F36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="AJ30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomRight" activeCell="AN53" sqref="AN53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4779,6 +4779,9 @@
       <c r="AL51" s="5">
         <v>4</v>
       </c>
+      <c r="AN51" s="5">
+        <v>2</v>
+      </c>
       <c r="AQ51" s="5">
         <v>2</v>
       </c>
@@ -4879,6 +4882,9 @@
       </c>
       <c r="AL53" s="5">
         <v>4</v>
+      </c>
+      <c r="AN53" s="5">
+        <v>2</v>
       </c>
       <c r="AQ53" s="5">
         <v>2</v>
@@ -7812,8 +7818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D169"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D61" sqref="D60:D61"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -11805,7 +11811,7 @@
   <dimension ref="A1:AG324"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="H5" sqref="H5:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>

</xml_diff>